<commit_message>
Add boundaries tab for full LWR case with h2 storage and export, optimizing h2 storage, htse and ft
</commit_message>
<xml_diff>
--- a/use_cases/2022_05/data/HERON_data.xlsx
+++ b/use_cases/2022_05/data/HERON_data.xlsx
@@ -8,20 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\garrm\projects\FORCE\use_cases\2022_05\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{257D98F4-FF1F-4C66-ADBC-B12F9A065227}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89336182-8F61-4B1C-9571-A115A087522F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="4" activeTab="8" xr2:uid="{3CE7F202-39F9-48AF-B0C7-575379157397}"/>
+    <workbookView xWindow="760" yWindow="760" windowWidth="14400" windowHeight="7360" firstSheet="1" activeTab="4" xr2:uid="{3CE7F202-39F9-48AF-B0C7-575379157397}"/>
   </bookViews>
   <sheets>
     <sheet name="MACRS" sheetId="1" r:id="rId1"/>
     <sheet name="HTSE" sheetId="2" r:id="rId2"/>
     <sheet name="FT" sheetId="7" r:id="rId3"/>
     <sheet name="Syn_base" sheetId="8" r:id="rId4"/>
-    <sheet name="FT_HTSE_combined" sheetId="9" r:id="rId5"/>
-    <sheet name="Capacity_Market" sheetId="3" r:id="rId6"/>
-    <sheet name="Transfer_rates" sheetId="4" r:id="rId7"/>
-    <sheet name="grid_sellall_test" sheetId="5" r:id="rId8"/>
-    <sheet name="grid_sellnothing_test" sheetId="6" r:id="rId9"/>
+    <sheet name="Boundaries" sheetId="10" r:id="rId5"/>
+    <sheet name="FT_HTSE_combined" sheetId="9" r:id="rId6"/>
+    <sheet name="Capacity_Market" sheetId="3" r:id="rId7"/>
+    <sheet name="Transfer_rates" sheetId="4" r:id="rId8"/>
+    <sheet name="grid_sellall_test" sheetId="5" r:id="rId9"/>
+    <sheet name="grid_sellnothing_test" sheetId="6" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="256">
   <si>
     <t>Source</t>
   </si>
@@ -745,6 +746,72 @@
   </si>
   <si>
     <t>Dan Wendt report</t>
+  </si>
+  <si>
+    <t>Components capacities optimization boundaries calculation</t>
+  </si>
+  <si>
+    <t>Fixed components</t>
+  </si>
+  <si>
+    <t>Purpose</t>
+  </si>
+  <si>
+    <t>Capacity negative when component is consuming a resource</t>
+  </si>
+  <si>
+    <t>Optimized components</t>
+  </si>
+  <si>
+    <t>Lower</t>
+  </si>
+  <si>
+    <t>Upper</t>
+  </si>
+  <si>
+    <t>kg-H2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Elec to H2 rate (HTSE) = 25.13 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Capacity  </t>
+  </si>
+  <si>
+    <t>Added to help optimization ($10000/kg-H2)</t>
+  </si>
+  <si>
+    <t>htse</t>
+  </si>
+  <si>
+    <t>ft</t>
+  </si>
+  <si>
+    <t>h2_export</t>
+  </si>
+  <si>
+    <t>turbine</t>
+  </si>
+  <si>
+    <t>ft_elec_consumption</t>
+  </si>
+  <si>
+    <t>elec_markte</t>
+  </si>
+  <si>
+    <t>jet_fuel_market</t>
+  </si>
+  <si>
+    <t>diesel_market</t>
+  </si>
+  <si>
+    <t>naphtha_market</t>
+  </si>
+  <si>
+    <t>h2_storage</t>
+  </si>
+  <si>
+    <t>10 kg initially stored, upper bound ~ 2h of storage for max capacity of FT</t>
   </si>
 </sst>
 </file>
@@ -1083,7 +1150,18 @@
     <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="12" xfId="3" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="4"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1095,17 +1173,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="4"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Bad" xfId="3" builtinId="27"/>
@@ -2614,10 +2681,10 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A2" s="50" t="s">
+      <c r="A2" s="55" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="50"/>
+      <c r="B2" s="55"/>
       <c r="C2" t="s">
         <v>4</v>
       </c>
@@ -2742,6 +2809,278 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8827ECA-5F74-4389-B5A8-A15818A92C9F}">
+  <dimension ref="A1:E42"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="31.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.6328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B1">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B3" s="2">
+        <v>10000</v>
+      </c>
+      <c r="C3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B4" s="2">
+        <v>10000</v>
+      </c>
+      <c r="C4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>71</v>
+      </c>
+      <c r="B5" s="2">
+        <v>10000</v>
+      </c>
+      <c r="C5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" t="s">
+        <v>82</v>
+      </c>
+      <c r="C8" t="s">
+        <v>83</v>
+      </c>
+      <c r="D8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>84</v>
+      </c>
+      <c r="B9" s="2">
+        <v>1000</v>
+      </c>
+      <c r="C9" s="2">
+        <v>750000</v>
+      </c>
+      <c r="D9" t="s">
+        <v>73</v>
+      </c>
+      <c r="E9" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="2">
+        <v>-750000</v>
+      </c>
+      <c r="C10" s="2">
+        <v>-1000</v>
+      </c>
+      <c r="D10" t="s">
+        <v>73</v>
+      </c>
+      <c r="E10" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="2">
+        <v>-100000</v>
+      </c>
+      <c r="C11" s="2">
+        <v>-1000</v>
+      </c>
+      <c r="D11" t="s">
+        <v>75</v>
+      </c>
+      <c r="E11" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>87</v>
+      </c>
+      <c r="B12" s="2">
+        <v>1000</v>
+      </c>
+      <c r="C12" s="2">
+        <v>500000</v>
+      </c>
+      <c r="D12" t="s">
+        <v>75</v>
+      </c>
+      <c r="E12" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="2">
+        <v>1000</v>
+      </c>
+      <c r="C13" s="2">
+        <v>200000</v>
+      </c>
+      <c r="D13" t="s">
+        <v>88</v>
+      </c>
+      <c r="E13" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>14</v>
+      </c>
+      <c r="B17" t="s">
+        <v>91</v>
+      </c>
+      <c r="C17" t="s">
+        <v>28</v>
+      </c>
+      <c r="D17" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>84</v>
+      </c>
+      <c r="B18" s="2">
+        <v>750000</v>
+      </c>
+      <c r="C18" t="s">
+        <v>73</v>
+      </c>
+      <c r="D18" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>17</v>
+      </c>
+      <c r="B19" s="2">
+        <v>-750000</v>
+      </c>
+      <c r="C19" t="s">
+        <v>73</v>
+      </c>
+      <c r="D19" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>15</v>
+      </c>
+      <c r="B20" s="2">
+        <v>-100000</v>
+      </c>
+      <c r="C20" t="s">
+        <v>75</v>
+      </c>
+      <c r="D20" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>16</v>
+      </c>
+      <c r="B22" s="2">
+        <v>1000</v>
+      </c>
+      <c r="C22" t="s">
+        <v>88</v>
+      </c>
+      <c r="D22" t="s">
+        <v>64</v>
+      </c>
+      <c r="E22" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="42" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E42" t="s">
+        <v>94</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -5149,28 +5488,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="50" t="s">
         <v>220</v>
       </c>
-      <c r="B1" s="50" t="s">
+      <c r="B1" s="55" t="s">
         <v>219</v>
       </c>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="54"/>
+      <c r="C1" s="55"/>
+      <c r="D1" s="55"/>
+      <c r="E1" s="55"/>
+      <c r="F1" s="50"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="55" t="s">
+      <c r="A2" s="51" t="s">
         <v>84</v>
       </c>
-      <c r="B2" s="56">
+      <c r="B2" s="52">
         <v>50</v>
       </c>
-      <c r="C2" s="56">
+      <c r="C2" s="52">
         <v>300</v>
       </c>
-      <c r="D2" s="57">
+      <c r="D2" s="53">
         <v>1000</v>
       </c>
     </row>
@@ -5195,11 +5534,11 @@
       <c r="A4" s="22" t="s">
         <v>169</v>
       </c>
-      <c r="B4" s="58">
+      <c r="B4" s="56">
         <v>-14.9</v>
       </c>
-      <c r="C4" s="58"/>
-      <c r="D4" s="59"/>
+      <c r="C4" s="56"/>
+      <c r="D4" s="57"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="22" t="s">
@@ -5257,6 +5596,209 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9241F20-95C4-42A2-B03A-23B9DD4DBFA3}">
+  <dimension ref="A1:E17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>236</v>
+      </c>
+      <c r="B1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>226</v>
+      </c>
+      <c r="B2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>179</v>
+      </c>
+      <c r="B4" t="s">
+        <v>243</v>
+      </c>
+      <c r="C4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>248</v>
+      </c>
+      <c r="B5">
+        <v>1000</v>
+      </c>
+      <c r="C5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>249</v>
+      </c>
+      <c r="B6">
+        <v>14.9</v>
+      </c>
+      <c r="C6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>250</v>
+      </c>
+      <c r="B7" s="2">
+        <v>-9.9999999999999997E+199</v>
+      </c>
+      <c r="C7" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>251</v>
+      </c>
+      <c r="B8" s="2">
+        <v>-9.9999999999999997E+199</v>
+      </c>
+      <c r="C8" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>252</v>
+      </c>
+      <c r="B9" s="2">
+        <v>-9.9999999999999997E+199</v>
+      </c>
+      <c r="C9" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>253</v>
+      </c>
+      <c r="B10" s="2">
+        <v>-9.9999999999999997E+199</v>
+      </c>
+      <c r="C10" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>247</v>
+      </c>
+      <c r="B11" s="2">
+        <v>9.9999999999999997E+199</v>
+      </c>
+      <c r="C11" t="s">
+        <v>241</v>
+      </c>
+      <c r="D11" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B12" s="2"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>179</v>
+      </c>
+      <c r="B14" t="s">
+        <v>239</v>
+      </c>
+      <c r="C14" t="s">
+        <v>240</v>
+      </c>
+      <c r="D14" t="s">
+        <v>28</v>
+      </c>
+      <c r="E14" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>245</v>
+      </c>
+      <c r="B15" s="2">
+        <v>-985.1</v>
+      </c>
+      <c r="C15">
+        <v>-10</v>
+      </c>
+      <c r="D15" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>246</v>
+      </c>
+      <c r="B16" s="2">
+        <v>-24650</v>
+      </c>
+      <c r="C16">
+        <v>-250</v>
+      </c>
+      <c r="D16" t="s">
+        <v>241</v>
+      </c>
+      <c r="E16" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>254</v>
+      </c>
+      <c r="B17">
+        <v>0</v>
+      </c>
+      <c r="C17">
+        <v>50000</v>
+      </c>
+      <c r="D17" t="s">
+        <v>241</v>
+      </c>
+      <c r="E17" t="s">
+        <v>255</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9120567B-0376-BC4D-A254-A4551F910A7D}">
   <dimension ref="A1:I28"/>
   <sheetViews>
@@ -5302,15 +5844,15 @@
       <c r="A5" t="s">
         <v>175</v>
       </c>
-      <c r="B5" s="51" t="s">
+      <c r="B5" s="58" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="52"/>
-      <c r="D5" s="52"/>
-      <c r="E5" s="52"/>
-      <c r="F5" s="52"/>
-      <c r="G5" s="52"/>
-      <c r="H5" s="53"/>
+      <c r="C5" s="59"/>
+      <c r="D5" s="59"/>
+      <c r="E5" s="59"/>
+      <c r="F5" s="59"/>
+      <c r="G5" s="59"/>
+      <c r="H5" s="60"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B6" s="22" t="s">
@@ -5431,15 +5973,15 @@
       <c r="H11" s="41"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B12" s="51" t="s">
+      <c r="B12" s="58" t="s">
         <v>217</v>
       </c>
-      <c r="C12" s="52"/>
-      <c r="D12" s="52"/>
-      <c r="E12" s="52"/>
-      <c r="F12" s="52"/>
-      <c r="G12" s="52"/>
-      <c r="H12" s="53"/>
+      <c r="C12" s="59"/>
+      <c r="D12" s="59"/>
+      <c r="E12" s="59"/>
+      <c r="F12" s="59"/>
+      <c r="G12" s="59"/>
+      <c r="H12" s="60"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B13" s="22" t="s">
@@ -5570,16 +6112,16 @@
     </row>
     <row r="20" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="21" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A21" s="51" t="s">
+      <c r="A21" s="58" t="s">
         <v>209</v>
       </c>
-      <c r="B21" s="52"/>
-      <c r="C21" s="52"/>
-      <c r="D21" s="53"/>
-      <c r="G21" s="51" t="s">
+      <c r="B21" s="59"/>
+      <c r="C21" s="59"/>
+      <c r="D21" s="60"/>
+      <c r="G21" s="58" t="s">
         <v>214</v>
       </c>
-      <c r="H21" s="53"/>
+      <c r="H21" s="60"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22" s="22" t="s">
@@ -5723,7 +6265,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FC147DE-C2D1-4559-861B-2B8673B56208}">
   <dimension ref="A1:C15"/>
   <sheetViews>
@@ -5855,7 +6397,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{926ACCEB-6613-41C3-AB8E-7E632C9D30FD}">
   <dimension ref="A1:H19"/>
   <sheetViews>
@@ -5879,7 +6421,7 @@
       <c r="A2" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="60" t="s">
+      <c r="B2" s="54" t="s">
         <v>232</v>
       </c>
     </row>
@@ -5887,34 +6429,34 @@
       <c r="A3" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="60" t="s">
+      <c r="B3" s="54" t="s">
         <v>233</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B4" s="60"/>
+      <c r="B4" s="54"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A5" s="50" t="s">
+      <c r="A5" s="55" t="s">
         <v>61</v>
       </c>
-      <c r="B5" s="50"/>
-      <c r="C5" s="50"/>
-      <c r="D5" s="50"/>
-      <c r="E5" s="50"/>
-      <c r="F5" s="50"/>
-      <c r="G5" s="50"/>
+      <c r="B5" s="55"/>
+      <c r="C5" s="55"/>
+      <c r="D5" s="55"/>
+      <c r="E5" s="55"/>
+      <c r="F5" s="55"/>
+      <c r="G5" s="55"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A6" s="50" t="s">
+      <c r="A6" s="55" t="s">
         <v>62</v>
       </c>
-      <c r="B6" s="50"/>
-      <c r="C6" s="50"/>
-      <c r="D6" s="50"/>
-      <c r="E6" s="50"/>
-      <c r="F6" s="50"/>
-      <c r="G6" s="50"/>
+      <c r="B6" s="55"/>
+      <c r="C6" s="55"/>
+      <c r="D6" s="55"/>
+      <c r="E6" s="55"/>
+      <c r="F6" s="55"/>
+      <c r="G6" s="55"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
@@ -5986,15 +6528,15 @@
       <c r="H9" s="2"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A10" s="50" t="s">
+      <c r="A10" s="55" t="s">
         <v>68</v>
       </c>
-      <c r="B10" s="50"/>
-      <c r="C10" s="50"/>
-      <c r="D10" s="50"/>
-      <c r="E10" s="50"/>
-      <c r="F10" s="50"/>
-      <c r="G10" s="50"/>
+      <c r="B10" s="55"/>
+      <c r="C10" s="55"/>
+      <c r="D10" s="55"/>
+      <c r="E10" s="55"/>
+      <c r="F10" s="55"/>
+      <c r="G10" s="55"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
@@ -6072,22 +6614,22 @@
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A15" s="50" t="s">
+      <c r="A15" s="55" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="50"/>
-      <c r="C15" s="50"/>
-      <c r="D15" s="50"/>
-      <c r="E15" s="50"/>
-      <c r="F15" s="50"/>
-      <c r="G15" s="50"/>
+      <c r="B15" s="55"/>
+      <c r="C15" s="55"/>
+      <c r="D15" s="55"/>
+      <c r="E15" s="55"/>
+      <c r="F15" s="55"/>
+      <c r="G15" s="55"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A16" s="50" t="s">
+      <c r="A16" s="55" t="s">
         <v>62</v>
       </c>
-      <c r="B16" s="50"/>
-      <c r="C16" s="50"/>
+      <c r="B16" s="55"/>
+      <c r="C16" s="55"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
@@ -6101,11 +6643,11 @@
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A18" s="50" t="s">
+      <c r="A18" s="55" t="s">
         <v>68</v>
       </c>
-      <c r="B18" s="50"/>
-      <c r="C18" s="50"/>
+      <c r="B18" s="55"/>
+      <c r="C18" s="55"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
@@ -6137,7 +6679,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CD4092A-9167-4B1E-A144-D4BB7A88B529}">
   <dimension ref="A1:E22"/>
   <sheetViews>
@@ -6389,276 +6931,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8827ECA-5F74-4389-B5A8-A15818A92C9F}">
-  <dimension ref="A1:E42"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="31.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.6328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>77</v>
-      </c>
-      <c r="B1">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B2">
-        <v>0</v>
-      </c>
-      <c r="C2" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>69</v>
-      </c>
-      <c r="B3" s="2">
-        <v>10000</v>
-      </c>
-      <c r="C3" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>70</v>
-      </c>
-      <c r="B4" s="2">
-        <v>10000</v>
-      </c>
-      <c r="C4" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>71</v>
-      </c>
-      <c r="B5" s="2">
-        <v>10000</v>
-      </c>
-      <c r="C5" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" t="s">
-        <v>82</v>
-      </c>
-      <c r="C8" t="s">
-        <v>83</v>
-      </c>
-      <c r="D8" t="s">
-        <v>28</v>
-      </c>
-      <c r="E8" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>84</v>
-      </c>
-      <c r="B9" s="2">
-        <v>1000</v>
-      </c>
-      <c r="C9" s="2">
-        <v>750000</v>
-      </c>
-      <c r="D9" t="s">
-        <v>73</v>
-      </c>
-      <c r="E9" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>17</v>
-      </c>
-      <c r="B10" s="2">
-        <v>-750000</v>
-      </c>
-      <c r="C10" s="2">
-        <v>-1000</v>
-      </c>
-      <c r="D10" t="s">
-        <v>73</v>
-      </c>
-      <c r="E10" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>15</v>
-      </c>
-      <c r="B11" s="2">
-        <v>-100000</v>
-      </c>
-      <c r="C11" s="2">
-        <v>-1000</v>
-      </c>
-      <c r="D11" t="s">
-        <v>75</v>
-      </c>
-      <c r="E11" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>87</v>
-      </c>
-      <c r="B12" s="2">
-        <v>1000</v>
-      </c>
-      <c r="C12" s="2">
-        <v>500000</v>
-      </c>
-      <c r="D12" t="s">
-        <v>75</v>
-      </c>
-      <c r="E12" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>16</v>
-      </c>
-      <c r="B13" s="2">
-        <v>1000</v>
-      </c>
-      <c r="C13" s="2">
-        <v>200000</v>
-      </c>
-      <c r="D13" t="s">
-        <v>88</v>
-      </c>
-      <c r="E13" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
-        <v>14</v>
-      </c>
-      <c r="B17" t="s">
-        <v>91</v>
-      </c>
-      <c r="C17" t="s">
-        <v>28</v>
-      </c>
-      <c r="D17" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
-        <v>84</v>
-      </c>
-      <c r="B18" s="2">
-        <v>750000</v>
-      </c>
-      <c r="C18" t="s">
-        <v>73</v>
-      </c>
-      <c r="D18" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
-        <v>17</v>
-      </c>
-      <c r="B19" s="2">
-        <v>-750000</v>
-      </c>
-      <c r="C19" t="s">
-        <v>73</v>
-      </c>
-      <c r="D19" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
-        <v>15</v>
-      </c>
-      <c r="B20" s="2">
-        <v>-100000</v>
-      </c>
-      <c r="C20" t="s">
-        <v>75</v>
-      </c>
-      <c r="D20" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
-        <v>16</v>
-      </c>
-      <c r="B22" s="2">
-        <v>1000</v>
-      </c>
-      <c r="C22" t="s">
-        <v>88</v>
-      </c>
-      <c r="D22" t="s">
-        <v>64</v>
-      </c>
-      <c r="E22" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="42" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E42" t="s">
-        <v>94</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Compute capex cashflow values for combined FT+HTSE component with updated ANL data
</commit_message>
<xml_diff>
--- a/use_cases/2022_05/data/HERON_data.xlsx
+++ b/use_cases/2022_05/data/HERON_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/garrm/FORCE/use_cases/2022_05/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EC37530-4036-7A43-8CAB-BEE7BA6811C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C37CBB7E-D599-6D41-A368-A699A92DAEDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1540" yWindow="500" windowWidth="31900" windowHeight="19680" firstSheet="1" activeTab="2" xr2:uid="{3CE7F202-39F9-48AF-B0C7-575379157397}"/>
+    <workbookView xWindow="-30700" yWindow="2860" windowWidth="26980" windowHeight="15200" firstSheet="1" activeTab="6" xr2:uid="{3CE7F202-39F9-48AF-B0C7-575379157397}"/>
   </bookViews>
   <sheets>
     <sheet name="MACRS" sheetId="1" r:id="rId1"/>
@@ -19,11 +19,12 @@
     <sheet name="FT_old" sheetId="7" r:id="rId4"/>
     <sheet name="Syn_base" sheetId="8" r:id="rId5"/>
     <sheet name="Boundaries" sheetId="10" r:id="rId6"/>
-    <sheet name="FT_HTSE_combined" sheetId="9" r:id="rId7"/>
-    <sheet name="Capacity_Market" sheetId="3" r:id="rId8"/>
-    <sheet name="Transfer_rates" sheetId="4" r:id="rId9"/>
-    <sheet name="grid_sellall_test" sheetId="5" r:id="rId10"/>
-    <sheet name="grid_sellnothing_test" sheetId="6" r:id="rId11"/>
+    <sheet name="FT_HTSE_combined" sheetId="12" r:id="rId7"/>
+    <sheet name="FT_HTSE_combined_old" sheetId="9" r:id="rId8"/>
+    <sheet name="Capacity_Market" sheetId="3" r:id="rId9"/>
+    <sheet name="Transfer_rates" sheetId="4" r:id="rId10"/>
+    <sheet name="grid_sellall_test" sheetId="5" r:id="rId11"/>
+    <sheet name="grid_sellnothing_test" sheetId="6" r:id="rId12"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -45,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="489" uniqueCount="284">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="588" uniqueCount="291">
   <si>
     <t>Source</t>
   </si>
@@ -897,6 +898,27 @@
   </si>
   <si>
     <t>$(2020)</t>
+  </si>
+  <si>
+    <t>Case without h2 storage, HTSE and FT combined into 1 component, updated data from ANL</t>
+  </si>
+  <si>
+    <t>FT (capacity expressed in MW of corresponding HTSE)</t>
+  </si>
+  <si>
+    <t>htse_ft_capacity</t>
+  </si>
+  <si>
+    <t>scaling_factor_x</t>
+  </si>
+  <si>
+    <t>reference_driver</t>
+  </si>
+  <si>
+    <t>MW</t>
+  </si>
+  <si>
+    <t>reference_price</t>
   </si>
 </sst>
 </file>
@@ -1174,7 +1196,7 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1240,6 +1262,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="4"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1258,8 +1282,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Bad" xfId="3" builtinId="27"/>
@@ -3857,10 +3880,10 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="55" t="s">
+      <c r="A2" s="57" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="55"/>
+      <c r="B2" s="57"/>
       <c r="C2" t="s">
         <v>4</v>
       </c>
@@ -3989,6 +4012,288 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{926ACCEB-6613-41C3-AB8E-7E632C9D30FD}">
+  <dimension ref="A1:H19"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="54" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="54" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B4" s="54"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="57" t="s">
+        <v>61</v>
+      </c>
+      <c r="B5" s="57"/>
+      <c r="C5" s="57"/>
+      <c r="D5" s="57"/>
+      <c r="E5" s="57"/>
+      <c r="F5" s="57"/>
+      <c r="G5" s="57"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="57" t="s">
+        <v>62</v>
+      </c>
+      <c r="B6" s="57"/>
+      <c r="C6" s="57"/>
+      <c r="D6" s="57"/>
+      <c r="E6" s="57"/>
+      <c r="F6" s="57"/>
+      <c r="G6" s="57"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>63</v>
+      </c>
+      <c r="B7">
+        <v>1580</v>
+      </c>
+      <c r="C7" t="s">
+        <v>67</v>
+      </c>
+      <c r="D7" s="3">
+        <f>B7*1000/(24*3600)</f>
+        <v>18.287037037037038</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="F7" s="5">
+        <f>B7*1000/24</f>
+        <v>65833.333333333328</v>
+      </c>
+      <c r="G7" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>64</v>
+      </c>
+      <c r="B8">
+        <v>255</v>
+      </c>
+      <c r="C8" t="s">
+        <v>67</v>
+      </c>
+      <c r="D8" s="3">
+        <f>B8*1000/(24*3600)</f>
+        <v>2.9513888888888888</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="F8" s="5">
+        <f>B8*1000/24</f>
+        <v>10625</v>
+      </c>
+      <c r="G8" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>65</v>
+      </c>
+      <c r="B9">
+        <v>14.9</v>
+      </c>
+      <c r="C9" t="s">
+        <v>66</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="E9" t="s">
+        <v>96</v>
+      </c>
+      <c r="F9" s="2"/>
+      <c r="H9" s="2"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" s="57" t="s">
+        <v>68</v>
+      </c>
+      <c r="B10" s="57"/>
+      <c r="C10" s="57"/>
+      <c r="D10" s="57"/>
+      <c r="E10" s="57"/>
+      <c r="F10" s="57"/>
+      <c r="G10" s="57"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>69</v>
+      </c>
+      <c r="B11">
+        <v>176</v>
+      </c>
+      <c r="C11" t="s">
+        <v>67</v>
+      </c>
+      <c r="D11" s="3">
+        <f>B11*1000/(24*3600)</f>
+        <v>2.0370370370370372</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="F11" s="5">
+        <f>B11*1000/24</f>
+        <v>7333.333333333333</v>
+      </c>
+      <c r="G11" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>70</v>
+      </c>
+      <c r="B12">
+        <v>213</v>
+      </c>
+      <c r="C12" t="s">
+        <v>67</v>
+      </c>
+      <c r="D12" s="3">
+        <f t="shared" ref="D12:D13" si="0">B12*1000/(24*3600)</f>
+        <v>2.4652777777777777</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="F12" s="5">
+        <f t="shared" ref="F12:F13" si="1">B12*1000/24</f>
+        <v>8875</v>
+      </c>
+      <c r="G12" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>71</v>
+      </c>
+      <c r="B13">
+        <v>118</v>
+      </c>
+      <c r="C13" t="s">
+        <v>67</v>
+      </c>
+      <c r="D13" s="3">
+        <f t="shared" si="0"/>
+        <v>1.3657407407407407</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="F13" s="5">
+        <f t="shared" si="1"/>
+        <v>4916.666666666667</v>
+      </c>
+      <c r="G13" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" s="57" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" s="57"/>
+      <c r="C15" s="57"/>
+      <c r="D15" s="57"/>
+      <c r="E15" s="57"/>
+      <c r="F15" s="57"/>
+      <c r="G15" s="57"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" s="57" t="s">
+        <v>62</v>
+      </c>
+      <c r="B16" s="57"/>
+      <c r="C16" s="57"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>65</v>
+      </c>
+      <c r="B17">
+        <v>39.799999999999997</v>
+      </c>
+      <c r="C17" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" s="57" t="s">
+        <v>68</v>
+      </c>
+      <c r="B18" s="57"/>
+      <c r="C18" s="57"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>64</v>
+      </c>
+      <c r="B19" s="6">
+        <f>1/B17</f>
+        <v>2.5125628140703519E-2</v>
+      </c>
+      <c r="C19" t="s">
+        <v>76</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="A18:C18"/>
+    <mergeCell ref="A6:G6"/>
+    <mergeCell ref="A10:G10"/>
+    <mergeCell ref="A5:G5"/>
+    <mergeCell ref="A15:G15"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{D47EE4A2-649A-42B4-8738-DF2E48262124}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{49708E60-D8BD-48F2-8030-EEB685223FB9}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CD4092A-9167-4B1E-A144-D4BB7A88B529}">
   <dimension ref="A1:E22"/>
   <sheetViews>
@@ -4242,7 +4547,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8827ECA-5F74-4389-B5A8-A15818A92C9F}">
   <dimension ref="A1:E42"/>
   <sheetViews>
@@ -4693,8 +4998,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D919D22-7A01-ED42-B8B2-84358A3D7717}">
   <dimension ref="A1:K25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4761,7 +5066,7 @@
       <c r="A7" t="s">
         <v>262</v>
       </c>
-      <c r="B7" s="61">
+      <c r="B7" s="55">
         <v>1.9E-2</v>
       </c>
       <c r="H7" t="s">
@@ -4932,7 +5237,7 @@
       <c r="A21" t="s">
         <v>276</v>
       </c>
-      <c r="B21" s="62">
+      <c r="B21" s="56">
         <f>POWER(1+B7,4)*FT_old!C18</f>
         <v>7640007.3719816608</v>
       </c>
@@ -4954,7 +5259,7 @@
       <c r="A25" t="s">
         <v>276</v>
       </c>
-      <c r="B25" s="62">
+      <c r="B25" s="56">
         <f>POWER(1+B7,4)*FT_old!C16</f>
         <v>21732221.278079256</v>
       </c>
@@ -7200,12 +7505,12 @@
       <c r="A1" s="50" t="s">
         <v>220</v>
       </c>
-      <c r="B1" s="55" t="s">
+      <c r="B1" s="57" t="s">
         <v>219</v>
       </c>
-      <c r="C1" s="55"/>
-      <c r="D1" s="55"/>
-      <c r="E1" s="55"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
       <c r="F1" s="50"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -7243,11 +7548,11 @@
       <c r="A4" s="22" t="s">
         <v>169</v>
       </c>
-      <c r="B4" s="56">
+      <c r="B4" s="58">
         <v>-14.9</v>
       </c>
-      <c r="C4" s="56"/>
-      <c r="D4" s="57"/>
+      <c r="C4" s="58"/>
+      <c r="D4" s="59"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="22" t="s">
@@ -7508,11 +7813,519 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75BB7584-3066-8D4D-9480-F9C4BB723ACA}">
+  <dimension ref="A1:H31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="33.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>226</v>
+      </c>
+      <c r="B1" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B2" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>176</v>
+      </c>
+      <c r="B3" t="s">
+        <v>177</v>
+      </c>
+      <c r="C3" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>175</v>
+      </c>
+      <c r="B6" s="60" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="61"/>
+      <c r="D6" s="61"/>
+      <c r="E6" s="61"/>
+      <c r="F6" s="61"/>
+      <c r="G6" s="61"/>
+      <c r="H6" s="62"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B7" s="22" t="s">
+        <v>179</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>180</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="G7" s="12" t="s">
+        <v>181</v>
+      </c>
+      <c r="H7" s="23"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B8" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>183</v>
+      </c>
+      <c r="D8" s="12">
+        <v>1</v>
+      </c>
+      <c r="E8" s="12"/>
+      <c r="F8" s="12" t="s">
+        <v>184</v>
+      </c>
+      <c r="G8" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="H8" s="23"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B9" s="22" t="s">
+        <v>201</v>
+      </c>
+      <c r="C9" s="12"/>
+      <c r="D9" s="12">
+        <v>20</v>
+      </c>
+      <c r="E9" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="F9" s="12"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="23"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B10" s="22" t="s">
+        <v>185</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>186</v>
+      </c>
+      <c r="D10" s="12">
+        <v>-30320</v>
+      </c>
+      <c r="E10" s="12" t="s">
+        <v>187</v>
+      </c>
+      <c r="F10" s="12" t="s">
+        <v>188</v>
+      </c>
+      <c r="G10" s="12" t="s">
+        <v>189</v>
+      </c>
+      <c r="H10" s="23"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B11" s="22" t="s">
+        <v>190</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>191</v>
+      </c>
+      <c r="D11" s="12">
+        <v>-3.1680000000000001</v>
+      </c>
+      <c r="E11" s="12" t="s">
+        <v>192</v>
+      </c>
+      <c r="F11" s="12" t="s">
+        <v>193</v>
+      </c>
+      <c r="G11" s="12" t="s">
+        <v>189</v>
+      </c>
+      <c r="H11" s="23"/>
+    </row>
+    <row r="12" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="40" t="s">
+        <v>194</v>
+      </c>
+      <c r="C12" s="31" t="s">
+        <v>186</v>
+      </c>
+      <c r="D12" s="31">
+        <v>-27933.45</v>
+      </c>
+      <c r="E12" s="31" t="s">
+        <v>195</v>
+      </c>
+      <c r="F12" s="31" t="s">
+        <v>188</v>
+      </c>
+      <c r="G12" s="31" t="s">
+        <v>189</v>
+      </c>
+      <c r="H12" s="41"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B13" s="60" t="s">
+        <v>285</v>
+      </c>
+      <c r="C13" s="61"/>
+      <c r="D13" s="61"/>
+      <c r="E13" s="61"/>
+      <c r="F13" s="61"/>
+      <c r="G13" s="61"/>
+      <c r="H13" s="62"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B14" s="22" t="s">
+        <v>179</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>180</v>
+      </c>
+      <c r="D14" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="E14" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="F14" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="G14" s="12" t="s">
+        <v>181</v>
+      </c>
+      <c r="H14" s="23"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B15" s="22" t="s">
+        <v>196</v>
+      </c>
+      <c r="C15" s="12" t="s">
+        <v>286</v>
+      </c>
+      <c r="D15" s="12"/>
+      <c r="E15" s="47"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="12"/>
+      <c r="H15" s="23"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B16" s="22"/>
+      <c r="C16" s="49" t="s">
+        <v>288</v>
+      </c>
+      <c r="D16" s="49">
+        <v>400</v>
+      </c>
+      <c r="E16" s="47" t="s">
+        <v>289</v>
+      </c>
+      <c r="F16" s="12"/>
+      <c r="G16" s="12"/>
+      <c r="H16" s="23"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B17" s="22"/>
+      <c r="C17" s="49" t="s">
+        <v>290</v>
+      </c>
+      <c r="D17" s="12">
+        <f>FT!B15</f>
+        <v>158102945</v>
+      </c>
+      <c r="E17" s="63" t="s">
+        <v>283</v>
+      </c>
+      <c r="F17" s="49" t="s">
+        <v>184</v>
+      </c>
+      <c r="G17" s="49" t="s">
+        <v>200</v>
+      </c>
+      <c r="H17" s="23"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B18" s="22"/>
+      <c r="C18" s="49" t="s">
+        <v>287</v>
+      </c>
+      <c r="D18" s="49">
+        <v>0.626</v>
+      </c>
+      <c r="E18" s="47"/>
+      <c r="F18" s="12"/>
+      <c r="G18" s="12"/>
+      <c r="H18" s="23"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B19" s="22" t="s">
+        <v>201</v>
+      </c>
+      <c r="C19" s="12"/>
+      <c r="D19" s="12">
+        <v>20</v>
+      </c>
+      <c r="E19" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="F19" s="12"/>
+      <c r="G19" s="12"/>
+      <c r="H19" s="23"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B20" s="22" t="s">
+        <v>202</v>
+      </c>
+      <c r="C20" s="12">
+        <v>1</v>
+      </c>
+      <c r="D20" s="12">
+        <v>-27412351</v>
+      </c>
+      <c r="E20" s="12" t="s">
+        <v>203</v>
+      </c>
+      <c r="F20" s="12" t="s">
+        <v>188</v>
+      </c>
+      <c r="G20" s="12" t="s">
+        <v>189</v>
+      </c>
+      <c r="H20" s="23"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B21" s="22" t="s">
+        <v>204</v>
+      </c>
+      <c r="C21" s="12">
+        <v>1</v>
+      </c>
+      <c r="D21" s="12">
+        <v>-9636868</v>
+      </c>
+      <c r="E21" s="12" t="s">
+        <v>203</v>
+      </c>
+      <c r="F21" s="12" t="s">
+        <v>188</v>
+      </c>
+      <c r="G21" s="12" t="s">
+        <v>189</v>
+      </c>
+      <c r="H21" s="23"/>
+    </row>
+    <row r="22" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="48" t="s">
+        <v>207</v>
+      </c>
+      <c r="C22" s="31" t="s">
+        <v>205</v>
+      </c>
+      <c r="D22" s="31">
+        <v>0.13100999999999999</v>
+      </c>
+      <c r="E22" s="31" t="s">
+        <v>206</v>
+      </c>
+      <c r="F22" s="31" t="s">
+        <v>193</v>
+      </c>
+      <c r="G22" s="31" t="s">
+        <v>189</v>
+      </c>
+      <c r="H22" s="41"/>
+    </row>
+    <row r="23" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A24" s="60" t="s">
+        <v>209</v>
+      </c>
+      <c r="B24" s="61"/>
+      <c r="C24" s="61"/>
+      <c r="D24" s="62"/>
+      <c r="G24" s="60" t="s">
+        <v>214</v>
+      </c>
+      <c r="H24" s="62"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A25" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="B25" s="12" t="s">
+        <v>210</v>
+      </c>
+      <c r="C25" s="12" t="s">
+        <v>208</v>
+      </c>
+      <c r="D25" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="G25" s="22" t="s">
+        <v>210</v>
+      </c>
+      <c r="H25" s="23" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A26" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="B26" s="12" t="s">
+        <v>174</v>
+      </c>
+      <c r="C26" s="12">
+        <v>-1</v>
+      </c>
+      <c r="D26" s="23" t="s">
+        <v>215</v>
+      </c>
+      <c r="G26" s="22" t="s">
+        <v>174</v>
+      </c>
+      <c r="H26" s="45">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A27" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="B27" s="12" t="s">
+        <v>205</v>
+      </c>
+      <c r="C27" s="12">
+        <v>25.13</v>
+      </c>
+      <c r="D27" s="23" t="s">
+        <v>216</v>
+      </c>
+      <c r="G27" s="22" t="s">
+        <v>211</v>
+      </c>
+      <c r="H27" s="45">
+        <f>(C29/ABS(C$28))*(C$27)</f>
+        <v>17.377632075471695</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A28" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="B28" s="12" t="s">
+        <v>205</v>
+      </c>
+      <c r="C28" s="12">
+        <v>-1.06</v>
+      </c>
+      <c r="D28" s="23" t="s">
+        <v>216</v>
+      </c>
+      <c r="G28" s="22" t="s">
+        <v>212</v>
+      </c>
+      <c r="H28" s="45">
+        <f>(C30/ABS(C$28))*(C$27)</f>
+        <v>21.052301886792449</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="B29" s="12" t="s">
+        <v>211</v>
+      </c>
+      <c r="C29" s="12">
+        <v>0.73299999999999998</v>
+      </c>
+      <c r="D29" s="23" t="s">
+        <v>216</v>
+      </c>
+      <c r="G29" s="40" t="s">
+        <v>213</v>
+      </c>
+      <c r="H29" s="46">
+        <f>(C31/ABS(C$28))*(C$27)</f>
+        <v>11.664113207547167</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A30" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="B30" s="12" t="s">
+        <v>212</v>
+      </c>
+      <c r="C30" s="12">
+        <v>0.88800000000000001</v>
+      </c>
+      <c r="D30" s="23" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="40" t="s">
+        <v>15</v>
+      </c>
+      <c r="B31" s="31" t="s">
+        <v>213</v>
+      </c>
+      <c r="C31" s="31">
+        <v>0.49199999999999999</v>
+      </c>
+      <c r="D31" s="41" t="s">
+        <v>216</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="B6:H6"/>
+    <mergeCell ref="B13:H13"/>
+    <mergeCell ref="A24:D24"/>
+    <mergeCell ref="G24:H24"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9120567B-0376-BC4D-A254-A4551F910A7D}">
   <dimension ref="A1:I28"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="A21" sqref="A21:H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7553,15 +8366,15 @@
       <c r="A5" t="s">
         <v>175</v>
       </c>
-      <c r="B5" s="58" t="s">
+      <c r="B5" s="60" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="59"/>
-      <c r="D5" s="59"/>
-      <c r="E5" s="59"/>
-      <c r="F5" s="59"/>
-      <c r="G5" s="59"/>
-      <c r="H5" s="60"/>
+      <c r="C5" s="61"/>
+      <c r="D5" s="61"/>
+      <c r="E5" s="61"/>
+      <c r="F5" s="61"/>
+      <c r="G5" s="61"/>
+      <c r="H5" s="62"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B6" s="22" t="s">
@@ -7682,15 +8495,15 @@
       <c r="H11" s="41"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B12" s="58" t="s">
+      <c r="B12" s="60" t="s">
         <v>217</v>
       </c>
-      <c r="C12" s="59"/>
-      <c r="D12" s="59"/>
-      <c r="E12" s="59"/>
-      <c r="F12" s="59"/>
-      <c r="G12" s="59"/>
-      <c r="H12" s="60"/>
+      <c r="C12" s="61"/>
+      <c r="D12" s="61"/>
+      <c r="E12" s="61"/>
+      <c r="F12" s="61"/>
+      <c r="G12" s="61"/>
+      <c r="H12" s="62"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B13" s="22" t="s">
@@ -7821,16 +8634,16 @@
     </row>
     <row r="20" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A21" s="58" t="s">
+      <c r="A21" s="60" t="s">
         <v>209</v>
       </c>
-      <c r="B21" s="59"/>
-      <c r="C21" s="59"/>
-      <c r="D21" s="60"/>
-      <c r="G21" s="58" t="s">
+      <c r="B21" s="61"/>
+      <c r="C21" s="61"/>
+      <c r="D21" s="62"/>
+      <c r="G21" s="60" t="s">
         <v>214</v>
       </c>
-      <c r="H21" s="60"/>
+      <c r="H21" s="62"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="22" t="s">
@@ -7974,7 +8787,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FC147DE-C2D1-4559-861B-2B8673B56208}">
   <dimension ref="A1:C15"/>
   <sheetViews>
@@ -8104,286 +8917,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{926ACCEB-6613-41C3-AB8E-7E632C9D30FD}">
-  <dimension ref="A1:H19"/>
-  <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.33203125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" s="54" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3" s="54" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B4" s="54"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="55" t="s">
-        <v>61</v>
-      </c>
-      <c r="B5" s="55"/>
-      <c r="C5" s="55"/>
-      <c r="D5" s="55"/>
-      <c r="E5" s="55"/>
-      <c r="F5" s="55"/>
-      <c r="G5" s="55"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="55" t="s">
-        <v>62</v>
-      </c>
-      <c r="B6" s="55"/>
-      <c r="C6" s="55"/>
-      <c r="D6" s="55"/>
-      <c r="E6" s="55"/>
-      <c r="F6" s="55"/>
-      <c r="G6" s="55"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>63</v>
-      </c>
-      <c r="B7">
-        <v>1580</v>
-      </c>
-      <c r="C7" t="s">
-        <v>67</v>
-      </c>
-      <c r="D7" s="3">
-        <f>B7*1000/(24*3600)</f>
-        <v>18.287037037037038</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="F7" s="5">
-        <f>B7*1000/24</f>
-        <v>65833.333333333328</v>
-      </c>
-      <c r="G7" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>64</v>
-      </c>
-      <c r="B8">
-        <v>255</v>
-      </c>
-      <c r="C8" t="s">
-        <v>67</v>
-      </c>
-      <c r="D8" s="3">
-        <f>B8*1000/(24*3600)</f>
-        <v>2.9513888888888888</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="F8" s="5">
-        <f>B8*1000/24</f>
-        <v>10625</v>
-      </c>
-      <c r="G8" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>65</v>
-      </c>
-      <c r="B9">
-        <v>14.9</v>
-      </c>
-      <c r="C9" t="s">
-        <v>66</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="E9" t="s">
-        <v>96</v>
-      </c>
-      <c r="F9" s="2"/>
-      <c r="H9" s="2"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" s="55" t="s">
-        <v>68</v>
-      </c>
-      <c r="B10" s="55"/>
-      <c r="C10" s="55"/>
-      <c r="D10" s="55"/>
-      <c r="E10" s="55"/>
-      <c r="F10" s="55"/>
-      <c r="G10" s="55"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>69</v>
-      </c>
-      <c r="B11">
-        <v>176</v>
-      </c>
-      <c r="C11" t="s">
-        <v>67</v>
-      </c>
-      <c r="D11" s="3">
-        <f>B11*1000/(24*3600)</f>
-        <v>2.0370370370370372</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="F11" s="5">
-        <f>B11*1000/24</f>
-        <v>7333.333333333333</v>
-      </c>
-      <c r="G11" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>70</v>
-      </c>
-      <c r="B12">
-        <v>213</v>
-      </c>
-      <c r="C12" t="s">
-        <v>67</v>
-      </c>
-      <c r="D12" s="3">
-        <f t="shared" ref="D12:D13" si="0">B12*1000/(24*3600)</f>
-        <v>2.4652777777777777</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="F12" s="5">
-        <f t="shared" ref="F12:F13" si="1">B12*1000/24</f>
-        <v>8875</v>
-      </c>
-      <c r="G12" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>71</v>
-      </c>
-      <c r="B13">
-        <v>118</v>
-      </c>
-      <c r="C13" t="s">
-        <v>67</v>
-      </c>
-      <c r="D13" s="3">
-        <f t="shared" si="0"/>
-        <v>1.3657407407407407</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="F13" s="5">
-        <f t="shared" si="1"/>
-        <v>4916.666666666667</v>
-      </c>
-      <c r="G13" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A15" s="55" t="s">
-        <v>17</v>
-      </c>
-      <c r="B15" s="55"/>
-      <c r="C15" s="55"/>
-      <c r="D15" s="55"/>
-      <c r="E15" s="55"/>
-      <c r="F15" s="55"/>
-      <c r="G15" s="55"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A16" s="55" t="s">
-        <v>62</v>
-      </c>
-      <c r="B16" s="55"/>
-      <c r="C16" s="55"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>65</v>
-      </c>
-      <c r="B17">
-        <v>39.799999999999997</v>
-      </c>
-      <c r="C17" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" s="55" t="s">
-        <v>68</v>
-      </c>
-      <c r="B18" s="55"/>
-      <c r="C18" s="55"/>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>64</v>
-      </c>
-      <c r="B19" s="6">
-        <f>1/B17</f>
-        <v>2.5125628140703519E-2</v>
-      </c>
-      <c r="C19" t="s">
-        <v>76</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="A16:C16"/>
-    <mergeCell ref="A18:C18"/>
-    <mergeCell ref="A6:G6"/>
-    <mergeCell ref="A10:G10"/>
-    <mergeCell ref="A5:G5"/>
-    <mergeCell ref="A15:G15"/>
-  </mergeCells>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{D47EE4A2-649A-42B4-8738-DF2E48262124}"/>
-    <hyperlink ref="B3" r:id="rId2" xr:uid="{49708E60-D8BD-48F2-8030-EEB685223FB9}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Wrong formula for delta NPV calculation
</commit_message>
<xml_diff>
--- a/use_cases/2022_05/data/HERON_data.xlsx
+++ b/use_cases/2022_05/data/HERON_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/garrm/FORCE/use_cases/2022_05/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C37CBB7E-D599-6D41-A368-A699A92DAEDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DDC9A8A-610D-A74D-9C20-C8DF193590F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-30700" yWindow="2860" windowWidth="26980" windowHeight="15200" firstSheet="1" activeTab="6" xr2:uid="{3CE7F202-39F9-48AF-B0C7-575379157397}"/>
   </bookViews>
@@ -930,7 +930,7 @@
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -981,6 +981,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Menlo"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -1196,7 +1202,7 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1283,6 +1289,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Bad" xfId="3" builtinId="27"/>
@@ -7823,6 +7830,7 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="33.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -8060,8 +8068,8 @@
         <v>290</v>
       </c>
       <c r="D17" s="12">
-        <f>FT!B15</f>
-        <v>158102945</v>
+        <f>-FT!B15</f>
+        <v>-158102945</v>
       </c>
       <c r="E17" s="63" t="s">
         <v>283</v>
@@ -8109,8 +8117,8 @@
       <c r="C20" s="12">
         <v>1</v>
       </c>
-      <c r="D20" s="12">
-        <v>-27412351</v>
+      <c r="D20" s="64">
+        <v>-21732221</v>
       </c>
       <c r="E20" s="12" t="s">
         <v>203</v>

</xml_diff>

<commit_message>
Add parallel run info
</commit_message>
<xml_diff>
--- a/use_cases/2022_05/data/HERON_data.xlsx
+++ b/use_cases/2022_05/data/HERON_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/garrm/FORCE/use_cases/2022_05/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DDC9A8A-610D-A74D-9C20-C8DF193590F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16041B77-245B-6446-A565-87CC7CE80620}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-30700" yWindow="2860" windowWidth="26980" windowHeight="15200" firstSheet="1" activeTab="6" xr2:uid="{3CE7F202-39F9-48AF-B0C7-575379157397}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20200" activeTab="9" xr2:uid="{3CE7F202-39F9-48AF-B0C7-575379157397}"/>
   </bookViews>
   <sheets>
     <sheet name="MACRS" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="588" uniqueCount="291">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="589" uniqueCount="292">
   <si>
     <t>Source</t>
   </si>
@@ -919,6 +919,9 @@
   </si>
   <si>
     <t>reference_price</t>
+  </si>
+  <si>
+    <t>kg-H2/MWh</t>
   </si>
 </sst>
 </file>
@@ -1202,7 +1205,7 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1218,17 +1221,10 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -1239,41 +1235,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="2" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="2" applyBorder="1"/>
-    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="12" xfId="3" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="4"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1288,8 +1271,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Bad" xfId="3" builtinId="27"/>
@@ -3887,10 +3868,10 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="57" t="s">
+      <c r="A2" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="57"/>
+      <c r="B2" s="44"/>
       <c r="C2" t="s">
         <v>4</v>
       </c>
@@ -4020,10 +4001,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{926ACCEB-6613-41C3-AB8E-7E632C9D30FD}">
-  <dimension ref="A1:H19"/>
+  <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4042,7 +4023,7 @@
       <c r="A2" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="54" t="s">
+      <c r="B2" s="40" t="s">
         <v>232</v>
       </c>
     </row>
@@ -4050,34 +4031,34 @@
       <c r="A3" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="54" t="s">
+      <c r="B3" s="40" t="s">
         <v>233</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B4" s="54"/>
+      <c r="B4" s="40"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="57" t="s">
+      <c r="A5" s="44" t="s">
         <v>61</v>
       </c>
-      <c r="B5" s="57"/>
-      <c r="C5" s="57"/>
-      <c r="D5" s="57"/>
-      <c r="E5" s="57"/>
-      <c r="F5" s="57"/>
-      <c r="G5" s="57"/>
+      <c r="B5" s="44"/>
+      <c r="C5" s="44"/>
+      <c r="D5" s="44"/>
+      <c r="E5" s="44"/>
+      <c r="F5" s="44"/>
+      <c r="G5" s="44"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="57" t="s">
+      <c r="A6" s="44" t="s">
         <v>62</v>
       </c>
-      <c r="B6" s="57"/>
-      <c r="C6" s="57"/>
-      <c r="D6" s="57"/>
-      <c r="E6" s="57"/>
-      <c r="F6" s="57"/>
-      <c r="G6" s="57"/>
+      <c r="B6" s="44"/>
+      <c r="C6" s="44"/>
+      <c r="D6" s="44"/>
+      <c r="E6" s="44"/>
+      <c r="F6" s="44"/>
+      <c r="G6" s="44"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
@@ -4149,15 +4130,15 @@
       <c r="H9" s="2"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" s="57" t="s">
+      <c r="A10" s="44" t="s">
         <v>68</v>
       </c>
-      <c r="B10" s="57"/>
-      <c r="C10" s="57"/>
-      <c r="D10" s="57"/>
-      <c r="E10" s="57"/>
-      <c r="F10" s="57"/>
-      <c r="G10" s="57"/>
+      <c r="B10" s="44"/>
+      <c r="C10" s="44"/>
+      <c r="D10" s="44"/>
+      <c r="E10" s="44"/>
+      <c r="F10" s="44"/>
+      <c r="G10" s="44"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
@@ -4235,22 +4216,22 @@
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A15" s="57" t="s">
+      <c r="A15" s="44" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="57"/>
-      <c r="C15" s="57"/>
-      <c r="D15" s="57"/>
-      <c r="E15" s="57"/>
-      <c r="F15" s="57"/>
-      <c r="G15" s="57"/>
+      <c r="B15" s="44"/>
+      <c r="C15" s="44"/>
+      <c r="D15" s="44"/>
+      <c r="E15" s="44"/>
+      <c r="F15" s="44"/>
+      <c r="G15" s="44"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A16" s="57" t="s">
+      <c r="A16" s="44" t="s">
         <v>62</v>
       </c>
-      <c r="B16" s="57"/>
-      <c r="C16" s="57"/>
+      <c r="B16" s="44"/>
+      <c r="C16" s="44"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
@@ -4264,11 +4245,11 @@
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" s="57" t="s">
+      <c r="A18" s="44" t="s">
         <v>68</v>
       </c>
-      <c r="B18" s="57"/>
-      <c r="C18" s="57"/>
+      <c r="B18" s="44"/>
+      <c r="C18" s="44"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
@@ -4280,6 +4261,15 @@
       </c>
       <c r="C19" t="s">
         <v>76</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B20">
+        <f>B19*1000</f>
+        <v>25.125628140703519</v>
+      </c>
+      <c r="C20" t="s">
+        <v>291</v>
       </c>
     </row>
   </sheetData>
@@ -4850,144 +4840,144 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="19" t="s">
+      <c r="C2" s="16" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="16">
+      <c r="B3" s="13">
         <v>36.799999999999997</v>
       </c>
-      <c r="C3" s="23" t="s">
+      <c r="C3" s="20" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="22"/>
-      <c r="B4" s="16">
+      <c r="A4" s="19"/>
+      <c r="B4" s="13">
         <f>1/B3</f>
         <v>2.7173913043478264E-2</v>
       </c>
-      <c r="C4" s="23" t="s">
+      <c r="C4" s="20" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="22" t="s">
+      <c r="A5" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="12">
+      <c r="B5">
         <v>6.4</v>
       </c>
-      <c r="C5" s="23" t="s">
+      <c r="C5" s="20" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="22" t="s">
+      <c r="A6" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="B6" s="12">
+      <c r="B6">
         <v>590</v>
       </c>
-      <c r="C6" s="23" t="s">
+      <c r="C6" s="20" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="22" t="s">
+      <c r="A7" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="B7" s="12">
+      <c r="B7">
         <v>763</v>
       </c>
-      <c r="C7" s="23" t="s">
+      <c r="C7" s="20" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="22" t="s">
+      <c r="A8" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="B8" s="12">
+      <c r="B8">
         <v>544</v>
       </c>
-      <c r="C8" s="23" t="s">
+      <c r="C8" s="20" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="22" t="s">
+      <c r="A9" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="B9" s="16">
+      <c r="B9" s="13">
         <v>703</v>
       </c>
-      <c r="C9" s="23" t="s">
+      <c r="C9" s="20" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="22" t="s">
+      <c r="A10" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="B10" s="12">
+      <c r="B10">
         <v>20</v>
       </c>
-      <c r="C10" s="23" t="s">
+      <c r="C10" s="20" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" s="22" t="s">
+      <c r="A11" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="B11" s="16">
+      <c r="B11" s="13">
         <v>32.64</v>
       </c>
-      <c r="C11" s="23" t="s">
+      <c r="C11" s="20" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" s="22" t="s">
+      <c r="A12" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="B12" s="16">
+      <c r="B12" s="13">
         <v>3.41</v>
       </c>
-      <c r="C12" s="23" t="s">
+      <c r="C12" s="20" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" s="22" t="s">
+      <c r="A13" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="B13" s="12">
+      <c r="B13">
         <v>10</v>
       </c>
-      <c r="C13" s="23" t="s">
+      <c r="C13" s="20" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="40" t="s">
+      <c r="A14" s="23" t="s">
         <v>46</v>
       </c>
-      <c r="B14" s="32">
+      <c r="B14" s="25">
         <v>20</v>
       </c>
-      <c r="C14" s="41" t="s">
+      <c r="C14" s="26" t="s">
         <v>39</v>
       </c>
     </row>
@@ -5006,7 +4996,7 @@
   <dimension ref="A1:K25"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5073,7 +5063,7 @@
       <c r="A7" t="s">
         <v>262</v>
       </c>
-      <c r="B7" s="55">
+      <c r="B7" s="41">
         <v>1.9E-2</v>
       </c>
       <c r="H7" t="s">
@@ -5244,7 +5234,7 @@
       <c r="A21" t="s">
         <v>276</v>
       </c>
-      <c r="B21" s="56">
+      <c r="B21" s="42">
         <f>POWER(1+B7,4)*FT_old!C18</f>
         <v>7640007.3719816608</v>
       </c>
@@ -5266,7 +5256,7 @@
       <c r="A25" t="s">
         <v>276</v>
       </c>
-      <c r="B25" s="56">
+      <c r="B25" s="42">
         <f>POWER(1+B7,4)*FT_old!C16</f>
         <v>21732221.278079256</v>
       </c>
@@ -5308,252 +5298,250 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="15" t="s">
         <v>100</v>
       </c>
-      <c r="C2" s="18" t="s">
+      <c r="C2" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="D2" s="19" t="s">
+      <c r="D2" s="16" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A3" s="20" t="s">
+      <c r="A3" s="17" t="s">
         <v>102</v>
       </c>
       <c r="B3" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="C3" s="34">
+      <c r="C3" s="27">
         <v>257800644</v>
       </c>
-      <c r="D3" s="21" t="s">
+      <c r="D3" s="18" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A4" s="22" t="s">
+      <c r="A4" s="19" t="s">
         <v>103</v>
       </c>
       <c r="B4" s="11" t="s">
         <v>111</v>
       </c>
-      <c r="C4" s="35">
+      <c r="C4" s="28">
         <f>0.02*C3</f>
         <v>5156012.88</v>
       </c>
-      <c r="D4" s="23" t="s">
+      <c r="D4" s="20" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A5" s="22"/>
+      <c r="A5" s="19"/>
       <c r="B5" s="11" t="s">
         <v>109</v>
       </c>
-      <c r="C5" s="35">
+      <c r="C5" s="28">
         <f>0.1*C3</f>
         <v>25780064.400000002</v>
       </c>
-      <c r="D5" s="23" t="s">
+      <c r="D5" s="20" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A6" s="22"/>
+      <c r="A6" s="19"/>
       <c r="B6" s="11" t="s">
         <v>107</v>
       </c>
-      <c r="C6" s="35">
+      <c r="C6" s="28">
         <f>0.15*C3</f>
         <v>38670096.600000001</v>
       </c>
-      <c r="D6" s="23" t="s">
+      <c r="D6" s="20" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A7" s="22"/>
+      <c r="A7" s="19"/>
       <c r="B7" s="11" t="s">
         <v>114</v>
       </c>
-      <c r="C7" s="35">
+      <c r="C7" s="28">
         <v>12251143</v>
       </c>
-      <c r="D7" s="23" t="s">
+      <c r="D7" s="20" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A8" s="22"/>
+      <c r="A8" s="19"/>
       <c r="B8" s="11" t="s">
         <v>108</v>
       </c>
-      <c r="C8" s="35">
+      <c r="C8" s="28">
         <f>0.15*C3</f>
         <v>38670096.600000001</v>
       </c>
-      <c r="D8" s="23" t="s">
+      <c r="D8" s="20" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="22" t="s">
+      <c r="A9" s="19" t="s">
         <v>113</v>
       </c>
       <c r="B9" s="11"/>
-      <c r="C9" s="35">
+      <c r="C9" s="28">
         <f>SUM(C4:C8)</f>
         <v>120527413.47999999</v>
       </c>
-      <c r="D9" s="23" t="s">
+      <c r="D9" s="20" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A10" s="22" t="s">
+      <c r="A10" s="19" t="s">
         <v>104</v>
       </c>
       <c r="B10" s="11" t="s">
         <v>105</v>
       </c>
-      <c r="C10" s="35">
+      <c r="C10" s="28">
         <f>10*55036</f>
         <v>550360</v>
       </c>
-      <c r="D10" s="23" t="s">
+      <c r="D10" s="20" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="24" t="s">
+      <c r="A11" s="21" t="s">
         <v>112</v>
       </c>
-      <c r="B11" s="13" t="s">
+      <c r="B11" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="C11" s="36">
+      <c r="C11" s="29">
         <f>SUM(C3,C9,C10)</f>
         <v>378878417.48000002</v>
       </c>
-      <c r="D11" s="25" t="s">
+      <c r="D11" s="22" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A12" s="26" t="s">
+      <c r="A12" s="17" t="s">
         <v>115</v>
       </c>
-      <c r="B12" s="15" t="s">
+      <c r="B12" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="C12" s="34">
+      <c r="C12" s="27">
         <v>9607972</v>
       </c>
-      <c r="D12" s="27" t="s">
+      <c r="D12" s="18" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A13" s="28" t="s">
+      <c r="A13" s="19" t="s">
         <v>118</v>
       </c>
-      <c r="B13" s="14" t="s">
+      <c r="B13" s="11" t="s">
         <v>121</v>
       </c>
-      <c r="C13" s="35">
+      <c r="C13" s="28">
         <f>0.2*C12</f>
         <v>1921594.4000000001</v>
       </c>
-      <c r="D13" s="29" t="s">
+      <c r="D13" s="20" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A14" s="28" t="s">
+      <c r="A14" s="19" t="s">
         <v>119</v>
       </c>
-      <c r="B14" s="14" t="s">
+      <c r="B14" s="11" t="s">
         <v>120</v>
       </c>
-      <c r="C14" s="35">
+      <c r="C14" s="28">
         <f>0.02*C11</f>
         <v>7577568.3496000003</v>
       </c>
-      <c r="D14" s="29" t="s">
+      <c r="D14" s="20" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="28" t="s">
+      <c r="A15" s="19" t="s">
         <v>122</v>
       </c>
-      <c r="B15" s="12"/>
-      <c r="C15" s="35">
+      <c r="C15" s="28">
         <v>1049006</v>
       </c>
-      <c r="D15" s="29" t="s">
+      <c r="D15" s="20" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="28" t="s">
+      <c r="A16" s="19" t="s">
         <v>123</v>
       </c>
-      <c r="B16" s="12"/>
-      <c r="C16" s="37">
+      <c r="C16" s="30">
         <f>SUM(C12:C15)</f>
         <v>20156140.749600001</v>
       </c>
-      <c r="D16" s="29" t="s">
+      <c r="D16" s="20" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A17" s="26" t="s">
+      <c r="A17" s="17" t="s">
         <v>124</v>
       </c>
       <c r="B17" s="10"/>
-      <c r="C17" s="34">
+      <c r="C17" s="27">
         <v>7085933</v>
       </c>
-      <c r="D17" s="27" t="s">
+      <c r="D17" s="18" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A18" s="38" t="s">
+      <c r="A18" s="21" t="s">
         <v>125</v>
       </c>
-      <c r="B18" s="13"/>
-      <c r="C18" s="36">
+      <c r="B18" s="12"/>
+      <c r="C18" s="29">
         <f>C17</f>
         <v>7085933</v>
       </c>
-      <c r="D18" s="39" t="s">
+      <c r="D18" s="22" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="19" spans="1:13" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="30" t="s">
+      <c r="A19" s="23" t="s">
         <v>126</v>
       </c>
-      <c r="B19" s="31" t="s">
+      <c r="B19" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="C19" s="31">
+      <c r="C19" s="24">
         <v>20</v>
       </c>
-      <c r="D19" s="33" t="s">
+      <c r="D19" s="26" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A20" s="28" t="s">
+      <c r="A20" s="19" t="s">
         <v>0</v>
       </c>
       <c r="B20" t="s">
@@ -5626,7 +5614,7 @@
       <c r="A25" t="s">
         <v>132</v>
       </c>
-      <c r="B25" s="42">
+      <c r="B25" s="31">
         <v>11807922</v>
       </c>
       <c r="C25">
@@ -5635,39 +5623,39 @@
       <c r="D25">
         <v>0.65</v>
       </c>
-      <c r="E25" s="43">
+      <c r="E25" s="32">
         <f>$B25*POWER(E$24,$D25)</f>
         <v>4795506.4702437567</v>
       </c>
-      <c r="F25" s="43">
+      <c r="F25" s="32">
         <f>$B25*POWER(F$24,$D25)</f>
         <v>7524956.2358284583</v>
       </c>
-      <c r="G25" s="43">
+      <c r="G25" s="32">
         <f t="shared" ref="F25:M40" si="0">$B25*POWER(G$24,$D25)</f>
         <v>11807922</v>
       </c>
-      <c r="H25" s="43">
+      <c r="H25" s="32">
         <f t="shared" si="0"/>
         <v>13651016.264884572</v>
       </c>
-      <c r="I25" s="43">
+      <c r="I25" s="32">
         <f t="shared" si="0"/>
         <v>15368546.448911712</v>
       </c>
-      <c r="J25" s="43">
+      <c r="J25" s="32">
         <f t="shared" si="0"/>
         <v>18528615.660810392</v>
       </c>
-      <c r="K25" s="43">
+      <c r="K25" s="32">
         <f t="shared" si="0"/>
         <v>29074514.407025062</v>
       </c>
-      <c r="L25" s="43">
+      <c r="L25" s="32">
         <f t="shared" si="0"/>
         <v>33612744.821986459</v>
       </c>
-      <c r="M25" s="43">
+      <c r="M25" s="32">
         <f t="shared" si="0"/>
         <v>52744050.147983856</v>
       </c>
@@ -5676,7 +5664,7 @@
       <c r="A26" t="s">
         <v>133</v>
       </c>
-      <c r="B26" s="42">
+      <c r="B26" s="31">
         <v>17388504</v>
       </c>
       <c r="C26">
@@ -5685,39 +5673,39 @@
       <c r="D26">
         <v>0.8</v>
       </c>
-      <c r="E26" s="43">
+      <c r="E26" s="32">
         <f t="shared" ref="E26:M58" si="1">$B26*POWER(E$24,$D26)</f>
         <v>5736067.1461265292</v>
       </c>
-      <c r="F26" s="43">
+      <c r="F26" s="32">
         <f t="shared" si="0"/>
         <v>9987072.9703296833</v>
       </c>
-      <c r="G26" s="43">
+      <c r="G26" s="32">
         <f t="shared" si="0"/>
         <v>17388504</v>
       </c>
-      <c r="H26" s="43">
+      <c r="H26" s="32">
         <f t="shared" si="0"/>
         <v>20786924.085011322</v>
       </c>
-      <c r="I26" s="43">
+      <c r="I26" s="32">
         <f t="shared" si="0"/>
         <v>24051115.660847504</v>
       </c>
-      <c r="J26" s="43">
+      <c r="J26" s="32">
         <f t="shared" si="0"/>
         <v>30275143.904153816</v>
       </c>
-      <c r="K26" s="43">
+      <c r="K26" s="32">
         <f t="shared" si="0"/>
         <v>52712087.159264646</v>
       </c>
-      <c r="L26" s="43">
+      <c r="L26" s="32">
         <f t="shared" si="0"/>
         <v>63014170.40489132</v>
       </c>
-      <c r="M26" s="43">
+      <c r="M26" s="32">
         <f t="shared" si="0"/>
         <v>109714043.08323221</v>
       </c>
@@ -5726,7 +5714,7 @@
       <c r="A27" t="s">
         <v>134</v>
       </c>
-      <c r="B27" s="42">
+      <c r="B27" s="31">
         <v>2547995</v>
       </c>
       <c r="C27">
@@ -5735,39 +5723,39 @@
       <c r="D27">
         <v>0.6</v>
       </c>
-      <c r="E27" s="43">
+      <c r="E27" s="32">
         <f t="shared" si="1"/>
         <v>1109079.2412628538</v>
       </c>
-      <c r="F27" s="43">
+      <c r="F27" s="32">
         <f t="shared" si="0"/>
         <v>1681049.7795548902</v>
       </c>
-      <c r="G27" s="43">
+      <c r="G27" s="32">
         <f t="shared" si="0"/>
         <v>2547995</v>
       </c>
-      <c r="H27" s="43">
+      <c r="H27" s="32">
         <f t="shared" si="0"/>
         <v>2913027.4644639199</v>
       </c>
-      <c r="I27" s="43">
+      <c r="I27" s="32">
         <f t="shared" si="0"/>
         <v>3249775.2504720115</v>
       </c>
-      <c r="J27" s="43">
+      <c r="J27" s="32">
         <f t="shared" si="0"/>
         <v>3862038.2328856615</v>
       </c>
-      <c r="K27" s="43">
+      <c r="K27" s="32">
         <f t="shared" si="0"/>
         <v>5853755.3300813409</v>
       </c>
-      <c r="L27" s="43">
+      <c r="L27" s="32">
         <f t="shared" si="0"/>
         <v>6692379.7129817763</v>
       </c>
-      <c r="M27" s="43">
+      <c r="M27" s="32">
         <f t="shared" si="0"/>
         <v>10143750.800344583</v>
       </c>
@@ -5776,7 +5764,7 @@
       <c r="A28" t="s">
         <v>135</v>
       </c>
-      <c r="B28" s="42">
+      <c r="B28" s="31">
         <v>22972192</v>
       </c>
       <c r="C28">
@@ -5785,39 +5773,39 @@
       <c r="D28">
         <v>0.6</v>
       </c>
-      <c r="E28" s="43">
+      <c r="E28" s="32">
         <f t="shared" si="1"/>
         <v>9999227.3428733572</v>
       </c>
-      <c r="F28" s="43">
+      <c r="F28" s="32">
         <f t="shared" si="0"/>
         <v>15155994.535896897</v>
       </c>
-      <c r="G28" s="43">
+      <c r="G28" s="32">
         <f t="shared" si="0"/>
         <v>22972192</v>
       </c>
-      <c r="H28" s="43">
+      <c r="H28" s="32">
         <f t="shared" si="0"/>
         <v>26263248.638611279</v>
       </c>
-      <c r="I28" s="43">
+      <c r="I28" s="32">
         <f t="shared" si="0"/>
         <v>29299296.509879783</v>
       </c>
-      <c r="J28" s="43">
+      <c r="J28" s="32">
         <f t="shared" si="0"/>
         <v>34819331.983457632</v>
       </c>
-      <c r="K28" s="43">
+      <c r="K28" s="32">
         <f t="shared" si="0"/>
         <v>52776238.322152101</v>
       </c>
-      <c r="L28" s="43">
+      <c r="L28" s="32">
         <f t="shared" si="0"/>
         <v>60337101.016101778</v>
       </c>
-      <c r="M28" s="43">
+      <c r="M28" s="32">
         <f t="shared" si="0"/>
         <v>91453943.585316852</v>
       </c>
@@ -5826,7 +5814,7 @@
       <c r="A29" t="s">
         <v>136</v>
       </c>
-      <c r="B29" s="42">
+      <c r="B29" s="31">
         <v>6248204</v>
       </c>
       <c r="C29">
@@ -5835,39 +5823,39 @@
       <c r="D29">
         <v>0.6</v>
       </c>
-      <c r="E29" s="43">
+      <c r="E29" s="32">
         <f t="shared" si="1"/>
         <v>2719688.7558945478</v>
       </c>
-      <c r="F29" s="43">
+      <c r="F29" s="32">
         <f t="shared" si="0"/>
         <v>4122277.3030614201</v>
       </c>
-      <c r="G29" s="43">
+      <c r="G29" s="32">
         <f t="shared" si="0"/>
         <v>6248204</v>
       </c>
-      <c r="H29" s="43">
+      <c r="H29" s="32">
         <f t="shared" si="0"/>
         <v>7143338.1366813211</v>
       </c>
-      <c r="I29" s="43">
+      <c r="I29" s="32">
         <f t="shared" si="0"/>
         <v>7969112.4665080681</v>
       </c>
-      <c r="J29" s="43">
+      <c r="J29" s="32">
         <f t="shared" si="0"/>
         <v>9470506.3137365356</v>
       </c>
-      <c r="K29" s="43">
+      <c r="K29" s="32">
         <f t="shared" si="0"/>
         <v>14354603.312971789</v>
       </c>
-      <c r="L29" s="43">
+      <c r="L29" s="32">
         <f t="shared" si="0"/>
         <v>16411081.533586834</v>
       </c>
-      <c r="M29" s="43">
+      <c r="M29" s="32">
         <f t="shared" si="0"/>
         <v>24874548.15481044</v>
       </c>
@@ -5876,7 +5864,7 @@
       <c r="A30" t="s">
         <v>137</v>
       </c>
-      <c r="B30" s="42">
+      <c r="B30" s="31">
         <v>32995221</v>
       </c>
       <c r="C30">
@@ -5885,39 +5873,39 @@
       <c r="D30">
         <v>0.6</v>
       </c>
-      <c r="E30" s="43">
+      <c r="E30" s="32">
         <f t="shared" si="1"/>
         <v>14362004.113815052</v>
       </c>
-      <c r="F30" s="43">
+      <c r="F30" s="32">
         <f t="shared" si="0"/>
         <v>21768727.563599963</v>
       </c>
-      <c r="G30" s="43">
+      <c r="G30" s="32">
         <f t="shared" si="0"/>
         <v>32995221</v>
       </c>
-      <c r="H30" s="43">
+      <c r="H30" s="32">
         <f t="shared" si="0"/>
         <v>37722203.131896526</v>
       </c>
-      <c r="I30" s="43">
+      <c r="I30" s="32">
         <f t="shared" si="0"/>
         <v>42082913.266962603</v>
       </c>
-      <c r="J30" s="43">
+      <c r="J30" s="32">
         <f t="shared" si="0"/>
         <v>50011403.085371777</v>
       </c>
-      <c r="K30" s="43">
+      <c r="K30" s="32">
         <f t="shared" si="0"/>
         <v>75803112.170927256</v>
       </c>
-      <c r="L30" s="43">
+      <c r="L30" s="32">
         <f t="shared" si="0"/>
         <v>86662865.368947059</v>
       </c>
-      <c r="M30" s="43">
+      <c r="M30" s="32">
         <f t="shared" si="0"/>
         <v>131356340.74097335</v>
       </c>
@@ -5926,7 +5914,7 @@
       <c r="A31" t="s">
         <v>138</v>
       </c>
-      <c r="B31" s="42">
+      <c r="B31" s="31">
         <v>4186906</v>
       </c>
       <c r="C31">
@@ -5935,39 +5923,39 @@
       <c r="D31">
         <v>0.7</v>
       </c>
-      <c r="E31" s="43">
+      <c r="E31" s="32">
         <f t="shared" si="1"/>
         <v>1586540.6966554464</v>
       </c>
-      <c r="F31" s="43">
+      <c r="F31" s="32">
         <f t="shared" si="0"/>
         <v>2577342.9655501549</v>
       </c>
-      <c r="G31" s="43">
+      <c r="G31" s="32">
         <f t="shared" si="0"/>
         <v>4186906</v>
       </c>
-      <c r="H31" s="43">
+      <c r="H31" s="32">
         <f t="shared" si="0"/>
         <v>4894746.672099025</v>
       </c>
-      <c r="I31" s="43">
+      <c r="I31" s="32">
         <f t="shared" si="0"/>
         <v>5561053.740726185</v>
       </c>
-      <c r="J31" s="43">
+      <c r="J31" s="32">
         <f t="shared" si="0"/>
         <v>6801648.8636366008</v>
       </c>
-      <c r="K31" s="43">
+      <c r="K31" s="32">
         <f t="shared" si="0"/>
         <v>11049311.17732499</v>
       </c>
-      <c r="L31" s="43">
+      <c r="L31" s="32">
         <f t="shared" si="0"/>
         <v>12917313.910127921</v>
       </c>
-      <c r="M31" s="43">
+      <c r="M31" s="32">
         <f t="shared" si="0"/>
         <v>20984238.355974279</v>
       </c>
@@ -5976,7 +5964,7 @@
       <c r="A32" t="s">
         <v>139</v>
       </c>
-      <c r="B32" s="42">
+      <c r="B32" s="31">
         <v>807728</v>
       </c>
       <c r="C32">
@@ -5985,39 +5973,39 @@
       <c r="D32">
         <v>0.7</v>
       </c>
-      <c r="E32" s="43">
+      <c r="E32" s="32">
         <f t="shared" si="1"/>
         <v>306071.67770857771</v>
       </c>
-      <c r="F32" s="43">
+      <c r="F32" s="32">
         <f t="shared" si="0"/>
         <v>497214.90735113126</v>
       </c>
-      <c r="G32" s="43">
+      <c r="G32" s="32">
         <f t="shared" si="0"/>
         <v>807728</v>
       </c>
-      <c r="H32" s="43">
+      <c r="H32" s="32">
         <f t="shared" si="0"/>
         <v>944282.94782858784</v>
       </c>
-      <c r="I32" s="43">
+      <c r="I32" s="32">
         <f t="shared" si="0"/>
         <v>1072825.3311369494</v>
       </c>
-      <c r="J32" s="43">
+      <c r="J32" s="32">
         <f t="shared" si="0"/>
         <v>1312158.0072080588</v>
       </c>
-      <c r="K32" s="43">
+      <c r="K32" s="32">
         <f t="shared" si="0"/>
         <v>2131606.9715055367</v>
       </c>
-      <c r="L32" s="43">
+      <c r="L32" s="32">
         <f t="shared" si="0"/>
         <v>2491977.6393355392</v>
       </c>
-      <c r="M32" s="43">
+      <c r="M32" s="32">
         <f t="shared" si="0"/>
         <v>4048229.6184328939</v>
       </c>
@@ -6026,7 +6014,7 @@
       <c r="A33" t="s">
         <v>147</v>
       </c>
-      <c r="B33" s="42">
+      <c r="B33" s="31">
         <v>75501</v>
       </c>
       <c r="C33">
@@ -6035,39 +6023,39 @@
       <c r="D33">
         <v>0.7</v>
       </c>
-      <c r="E33" s="43">
+      <c r="E33" s="32">
         <f t="shared" si="1"/>
         <v>28609.529122025393</v>
       </c>
-      <c r="F33" s="43">
+      <c r="F33" s="32">
         <f t="shared" si="0"/>
         <v>46476.317175977267</v>
       </c>
-      <c r="G33" s="43">
+      <c r="G33" s="32">
         <f t="shared" si="0"/>
         <v>75501</v>
       </c>
-      <c r="H33" s="43">
+      <c r="H33" s="32">
         <f t="shared" si="0"/>
         <v>88265.24132381966</v>
       </c>
-      <c r="I33" s="43">
+      <c r="I33" s="32">
         <f t="shared" si="0"/>
         <v>100280.52181696167</v>
       </c>
-      <c r="J33" s="43">
+      <c r="J33" s="32">
         <f t="shared" si="0"/>
         <v>122651.73635458427</v>
       </c>
-      <c r="K33" s="43">
+      <c r="K33" s="32">
         <f t="shared" si="0"/>
         <v>199248.33354252856</v>
       </c>
-      <c r="L33" s="43">
+      <c r="L33" s="32">
         <f t="shared" si="0"/>
         <v>232933.3683461172</v>
       </c>
-      <c r="M33" s="43">
+      <c r="M33" s="32">
         <f t="shared" si="0"/>
         <v>378401.37326092686</v>
       </c>
@@ -6076,7 +6064,7 @@
       <c r="A34" t="s">
         <v>140</v>
       </c>
-      <c r="B34" s="42">
+      <c r="B34" s="31">
         <v>11461600</v>
       </c>
       <c r="C34">
@@ -6085,39 +6073,39 @@
       <c r="D34">
         <v>0.65</v>
       </c>
-      <c r="E34" s="43">
+      <c r="E34" s="32">
         <f t="shared" si="1"/>
         <v>4654856.0330383144</v>
       </c>
-      <c r="F34" s="43">
+      <c r="F34" s="32">
         <f t="shared" si="0"/>
         <v>7304252.0430412283</v>
       </c>
-      <c r="G34" s="43">
+      <c r="G34" s="32">
         <f t="shared" si="0"/>
         <v>11461600</v>
       </c>
-      <c r="H34" s="43">
+      <c r="H34" s="32">
         <f t="shared" si="0"/>
         <v>13250636.989438193</v>
       </c>
-      <c r="I34" s="43">
+      <c r="I34" s="32">
         <f t="shared" si="0"/>
         <v>14917792.646229072</v>
       </c>
-      <c r="J34" s="43">
+      <c r="J34" s="32">
         <f t="shared" si="0"/>
         <v>17985178.192906797</v>
       </c>
-      <c r="K34" s="43">
+      <c r="K34" s="32">
         <f t="shared" si="0"/>
         <v>28221769.615988184</v>
       </c>
-      <c r="L34" s="43">
+      <c r="L34" s="32">
         <f t="shared" si="0"/>
         <v>32626895.405616667</v>
       </c>
-      <c r="M34" s="43">
+      <c r="M34" s="32">
         <f t="shared" si="0"/>
         <v>51197086.5979748</v>
       </c>
@@ -6126,7 +6114,7 @@
       <c r="A35" t="s">
         <v>141</v>
       </c>
-      <c r="B35" s="42">
+      <c r="B35" s="31">
         <v>36681585</v>
       </c>
       <c r="C35">
@@ -6135,39 +6123,39 @@
       <c r="D35">
         <v>0.8</v>
       </c>
-      <c r="E35" s="43">
+      <c r="E35" s="32">
         <f t="shared" si="1"/>
         <v>12100410.396797085</v>
       </c>
-      <c r="F35" s="43">
+      <c r="F35" s="32">
         <f t="shared" si="0"/>
         <v>21068038.174091958</v>
       </c>
-      <c r="G35" s="43">
+      <c r="G35" s="32">
         <f t="shared" si="0"/>
         <v>36681585</v>
       </c>
-      <c r="H35" s="43">
+      <c r="H35" s="32">
         <f t="shared" si="0"/>
         <v>43850656.888763405</v>
       </c>
-      <c r="I35" s="43">
+      <c r="I35" s="32">
         <f t="shared" si="0"/>
         <v>50736569.601284206</v>
       </c>
-      <c r="J35" s="43">
+      <c r="J35" s="32">
         <f t="shared" si="0"/>
         <v>63866348.968689315</v>
       </c>
-      <c r="K35" s="43">
+      <c r="K35" s="32">
         <f t="shared" si="0"/>
         <v>111197772.14071864</v>
       </c>
-      <c r="L35" s="43">
+      <c r="L35" s="32">
         <f t="shared" si="0"/>
         <v>132930334.19732401</v>
       </c>
-      <c r="M35" s="43">
+      <c r="M35" s="32">
         <f t="shared" si="0"/>
         <v>231445154.62924495</v>
       </c>
@@ -6176,7 +6164,7 @@
       <c r="A36" t="s">
         <v>142</v>
       </c>
-      <c r="B36" s="42">
+      <c r="B36" s="31">
         <v>144155</v>
       </c>
       <c r="C36">
@@ -6185,39 +6173,39 @@
       <c r="D36">
         <v>0.6</v>
       </c>
-      <c r="E36" s="43">
+      <c r="E36" s="32">
         <f t="shared" si="1"/>
         <v>62747.108225976386</v>
       </c>
-      <c r="F36" s="43">
+      <c r="F36" s="32">
         <f t="shared" si="0"/>
         <v>95106.831438733279</v>
       </c>
-      <c r="G36" s="43">
+      <c r="G36" s="32">
         <f t="shared" si="0"/>
         <v>144155</v>
       </c>
-      <c r="H36" s="43">
+      <c r="H36" s="32">
         <f t="shared" si="0"/>
         <v>164807.02440145935</v>
       </c>
-      <c r="I36" s="43">
+      <c r="I36" s="32">
         <f t="shared" si="0"/>
         <v>183858.81888771086</v>
       </c>
-      <c r="J36" s="43">
+      <c r="J36" s="32">
         <f t="shared" si="0"/>
         <v>218498.12164530641</v>
       </c>
-      <c r="K36" s="43">
+      <c r="K36" s="32">
         <f t="shared" si="0"/>
         <v>331181.2227291952</v>
       </c>
-      <c r="L36" s="43">
+      <c r="L36" s="32">
         <f t="shared" si="0"/>
         <v>378627.11564382503</v>
       </c>
-      <c r="M36" s="43">
+      <c r="M36" s="32">
         <f t="shared" si="0"/>
         <v>573891.39171139395</v>
       </c>
@@ -6226,7 +6214,7 @@
       <c r="A37" t="s">
         <v>143</v>
       </c>
-      <c r="B37" s="42">
+      <c r="B37" s="31">
         <v>6595713</v>
       </c>
       <c r="C37">
@@ -6235,39 +6223,39 @@
       <c r="D37">
         <v>0.7</v>
       </c>
-      <c r="E37" s="43">
+      <c r="E37" s="32">
         <f t="shared" si="1"/>
         <v>2499307.8655119995</v>
       </c>
-      <c r="F37" s="43">
+      <c r="F37" s="32">
         <f t="shared" si="0"/>
         <v>4060137.6059882189</v>
       </c>
-      <c r="G37" s="43">
+      <c r="G37" s="32">
         <f t="shared" si="0"/>
         <v>6595713</v>
       </c>
-      <c r="H37" s="43">
+      <c r="H37" s="32">
         <f t="shared" si="0"/>
         <v>7710787.9319168562</v>
       </c>
-      <c r="I37" s="43">
+      <c r="I37" s="32">
         <f t="shared" si="0"/>
         <v>8760434.1849103682</v>
       </c>
-      <c r="J37" s="43">
+      <c r="J37" s="32">
         <f t="shared" si="0"/>
         <v>10714767.379855949</v>
       </c>
-      <c r="K37" s="43">
+      <c r="K37" s="32">
         <f t="shared" si="0"/>
         <v>17406190.961375237</v>
       </c>
-      <c r="L37" s="43">
+      <c r="L37" s="32">
         <f t="shared" si="0"/>
         <v>20348891.348912913</v>
       </c>
-      <c r="M37" s="43">
+      <c r="M37" s="32">
         <f t="shared" si="0"/>
         <v>33056871.522694372</v>
       </c>
@@ -6276,7 +6264,7 @@
       <c r="A38" t="s">
         <v>144</v>
       </c>
-      <c r="B38" s="42">
+      <c r="B38" s="31">
         <v>1626125</v>
       </c>
       <c r="C38">
@@ -6285,39 +6273,39 @@
       <c r="D38">
         <v>0.7</v>
       </c>
-      <c r="E38" s="43">
+      <c r="E38" s="32">
         <f t="shared" si="1"/>
         <v>616186.15042918036</v>
       </c>
-      <c r="F38" s="43">
+      <c r="F38" s="32">
         <f t="shared" si="0"/>
         <v>1000997.354575251</v>
       </c>
-      <c r="G38" s="43">
+      <c r="G38" s="32">
         <f t="shared" si="0"/>
         <v>1626125</v>
       </c>
-      <c r="H38" s="43">
+      <c r="H38" s="32">
         <f t="shared" si="0"/>
         <v>1901038.6027694501</v>
       </c>
-      <c r="I38" s="43">
+      <c r="I38" s="32">
         <f t="shared" si="0"/>
         <v>2159821.2413028539</v>
       </c>
-      <c r="J38" s="43">
+      <c r="J38" s="32">
         <f t="shared" si="0"/>
         <v>2641647.856049567</v>
       </c>
-      <c r="K38" s="43">
+      <c r="K38" s="32">
         <f t="shared" si="0"/>
         <v>4291369.6028111456</v>
       </c>
-      <c r="L38" s="43">
+      <c r="L38" s="32">
         <f t="shared" si="0"/>
         <v>5016870.9500778774</v>
       </c>
-      <c r="M38" s="43">
+      <c r="M38" s="32">
         <f t="shared" si="0"/>
         <v>8149930.9028214812</v>
       </c>
@@ -6326,7 +6314,7 @@
       <c r="A39" t="s">
         <v>145</v>
       </c>
-      <c r="B39" s="42">
+      <c r="B39" s="31">
         <v>980551</v>
       </c>
       <c r="C39">
@@ -6335,39 +6323,39 @@
       <c r="D39">
         <v>0.7</v>
       </c>
-      <c r="E39" s="43">
+      <c r="E39" s="32">
         <f t="shared" si="1"/>
         <v>371559.34875208436</v>
       </c>
-      <c r="F39" s="43">
+      <c r="F39" s="32">
         <f t="shared" si="0"/>
         <v>603599.94282488548</v>
       </c>
-      <c r="G39" s="43">
+      <c r="G39" s="32">
         <f t="shared" si="0"/>
         <v>980551</v>
       </c>
-      <c r="H39" s="43">
+      <c r="H39" s="32">
         <f t="shared" si="0"/>
         <v>1146323.5009511488</v>
       </c>
-      <c r="I39" s="43">
+      <c r="I39" s="32">
         <f t="shared" si="0"/>
         <v>1302369.0540276761</v>
       </c>
-      <c r="J39" s="43">
+      <c r="J39" s="32">
         <f t="shared" si="0"/>
         <v>1592909.7989990062</v>
       </c>
-      <c r="K39" s="43">
+      <c r="K39" s="32">
         <f t="shared" si="0"/>
         <v>2587689.6028325441</v>
       </c>
-      <c r="L39" s="43">
+      <c r="L39" s="32">
         <f t="shared" si="0"/>
         <v>3025165.8556198403</v>
       </c>
-      <c r="M39" s="43">
+      <c r="M39" s="32">
         <f t="shared" si="0"/>
         <v>4914396.4312045546</v>
       </c>
@@ -6376,7 +6364,7 @@
       <c r="A40" t="s">
         <v>146</v>
       </c>
-      <c r="B40" s="42">
+      <c r="B40" s="31">
         <v>123670</v>
       </c>
       <c r="C40">
@@ -6385,39 +6373,39 @@
       <c r="D40">
         <v>0.6</v>
       </c>
-      <c r="E40" s="43">
+      <c r="E40" s="32">
         <f t="shared" si="1"/>
         <v>53830.494081415833</v>
       </c>
-      <c r="F40" s="43">
+      <c r="F40" s="32">
         <f t="shared" si="0"/>
         <v>81591.771662641913</v>
       </c>
-      <c r="G40" s="43">
+      <c r="G40" s="32">
         <f t="shared" si="0"/>
         <v>123670</v>
       </c>
-      <c r="H40" s="43">
+      <c r="H40" s="32">
         <f t="shared" si="0"/>
         <v>141387.28942963114</v>
       </c>
-      <c r="I40" s="43">
+      <c r="I40" s="32">
         <f t="shared" si="0"/>
         <v>157731.74799239152</v>
       </c>
-      <c r="J40" s="43">
+      <c r="J40" s="32">
         <f t="shared" si="0"/>
         <v>187448.66778034091</v>
       </c>
-      <c r="K40" s="43">
+      <c r="K40" s="32">
         <f t="shared" si="0"/>
         <v>284119.05112496665</v>
       </c>
-      <c r="L40" s="43">
+      <c r="L40" s="32">
         <f t="shared" si="0"/>
         <v>324822.69357061386</v>
       </c>
-      <c r="M40" s="43">
+      <c r="M40" s="32">
         <f t="shared" si="0"/>
         <v>492339.1378235101</v>
       </c>
@@ -6426,7 +6414,7 @@
       <c r="A41" t="s">
         <v>148</v>
       </c>
-      <c r="B41" s="42">
+      <c r="B41" s="31">
         <v>718300</v>
       </c>
       <c r="C41">
@@ -6435,39 +6423,39 @@
       <c r="D41">
         <v>0.8</v>
       </c>
-      <c r="E41" s="43">
+      <c r="E41" s="32">
         <f t="shared" si="1"/>
         <v>236950.63307704253</v>
       </c>
-      <c r="F41" s="43">
+      <c r="F41" s="32">
         <f t="shared" si="1"/>
         <v>412555.01419718517</v>
       </c>
-      <c r="G41" s="43">
+      <c r="G41" s="32">
         <f t="shared" si="1"/>
         <v>718300</v>
       </c>
-      <c r="H41" s="43">
+      <c r="H41" s="32">
         <f t="shared" si="1"/>
         <v>858685.00074897939</v>
       </c>
-      <c r="I41" s="43">
+      <c r="I41" s="32">
         <f t="shared" si="1"/>
         <v>993525.16922598751</v>
       </c>
-      <c r="J41" s="43">
+      <c r="J41" s="32">
         <f t="shared" si="1"/>
         <v>1250632.939231212</v>
       </c>
-      <c r="K41" s="43">
+      <c r="K41" s="32">
         <f t="shared" si="1"/>
         <v>2177478.4194488376</v>
       </c>
-      <c r="L41" s="43">
+      <c r="L41" s="32">
         <f t="shared" si="1"/>
         <v>2603046.1620984436</v>
       </c>
-      <c r="M41" s="43">
+      <c r="M41" s="32">
         <f t="shared" si="1"/>
         <v>4532166.6054012291</v>
       </c>
@@ -6476,7 +6464,7 @@
       <c r="A42" t="s">
         <v>149</v>
       </c>
-      <c r="B42" s="42">
+      <c r="B42" s="31">
         <v>7495642</v>
       </c>
       <c r="C42">
@@ -6485,39 +6473,39 @@
       <c r="D42">
         <v>0.6</v>
       </c>
-      <c r="E42" s="43">
+      <c r="E42" s="32">
         <f t="shared" si="1"/>
         <v>3262667.6826830432</v>
       </c>
-      <c r="F42" s="43">
+      <c r="F42" s="32">
         <f t="shared" si="1"/>
         <v>4945279.4576607794</v>
       </c>
-      <c r="G42" s="43">
+      <c r="G42" s="32">
         <f t="shared" si="1"/>
         <v>7495642</v>
       </c>
-      <c r="H42" s="43">
+      <c r="H42" s="32">
         <f t="shared" si="1"/>
         <v>8569487.3850966208</v>
       </c>
-      <c r="I42" s="43">
+      <c r="I42" s="32">
         <f t="shared" si="1"/>
         <v>9560125.4547197036</v>
       </c>
-      <c r="J42" s="43">
+      <c r="J42" s="32">
         <f t="shared" si="1"/>
         <v>11361268.756031133</v>
       </c>
-      <c r="K42" s="43">
+      <c r="K42" s="32">
         <f t="shared" si="1"/>
         <v>17220463.270093374</v>
       </c>
-      <c r="L42" s="43">
+      <c r="L42" s="32">
         <f t="shared" si="1"/>
         <v>19687512.124856662</v>
       </c>
-      <c r="M42" s="43">
+      <c r="M42" s="32">
         <f t="shared" si="1"/>
         <v>29840688.281019572</v>
       </c>
@@ -6526,7 +6514,7 @@
       <c r="A43" t="s">
         <v>150</v>
       </c>
-      <c r="B43" s="42">
+      <c r="B43" s="31">
         <v>969104</v>
       </c>
       <c r="C43">
@@ -6535,39 +6523,39 @@
       <c r="D43">
         <v>0.7</v>
       </c>
-      <c r="E43" s="43">
+      <c r="E43" s="32">
         <f t="shared" si="1"/>
         <v>367221.74686787324</v>
       </c>
-      <c r="F43" s="43">
+      <c r="F43" s="32">
         <f t="shared" si="1"/>
         <v>596553.48777510587</v>
       </c>
-      <c r="G43" s="43">
+      <c r="G43" s="32">
         <f t="shared" si="1"/>
         <v>969104</v>
       </c>
-      <c r="H43" s="43">
+      <c r="H43" s="32">
         <f t="shared" si="1"/>
         <v>1132941.2647233671</v>
       </c>
-      <c r="I43" s="43">
+      <c r="I43" s="32">
         <f t="shared" si="1"/>
         <v>1287165.1344340448</v>
       </c>
-      <c r="J43" s="43">
+      <c r="J43" s="32">
         <f t="shared" si="1"/>
         <v>1574314.0926368264</v>
       </c>
-      <c r="K43" s="43">
+      <c r="K43" s="32">
         <f t="shared" si="1"/>
         <v>2557480.7887233095</v>
       </c>
-      <c r="L43" s="43">
+      <c r="L43" s="32">
         <f t="shared" si="1"/>
         <v>2989849.9224870605</v>
       </c>
-      <c r="M43" s="43">
+      <c r="M43" s="32">
         <f t="shared" si="1"/>
         <v>4857025.5285712406</v>
       </c>
@@ -6576,7 +6564,7 @@
       <c r="A44" t="s">
         <v>151</v>
       </c>
-      <c r="B44" s="42">
+      <c r="B44" s="31">
         <v>29456</v>
       </c>
       <c r="C44">
@@ -6585,39 +6573,39 @@
       <c r="D44">
         <v>0.7</v>
       </c>
-      <c r="E44" s="43">
+      <c r="E44" s="32">
         <f t="shared" si="1"/>
         <v>11161.736795782572</v>
       </c>
-      <c r="F44" s="43">
+      <c r="F44" s="32">
         <f t="shared" si="1"/>
         <v>18132.294919743927</v>
       </c>
-      <c r="G44" s="43">
+      <c r="G44" s="32">
         <f t="shared" si="1"/>
         <v>29456</v>
       </c>
-      <c r="H44" s="43">
+      <c r="H44" s="32">
         <f t="shared" si="1"/>
         <v>34435.847848828918</v>
       </c>
-      <c r="I44" s="43">
+      <c r="I44" s="32">
         <f t="shared" si="1"/>
         <v>39123.495723770851</v>
       </c>
-      <c r="J44" s="43">
+      <c r="J44" s="32">
         <f t="shared" si="1"/>
         <v>47851.413174138543</v>
       </c>
-      <c r="K44" s="43">
+      <c r="K44" s="32">
         <f t="shared" si="1"/>
         <v>77734.850039452736</v>
       </c>
-      <c r="L44" s="43">
+      <c r="L44" s="32">
         <f t="shared" si="1"/>
         <v>90876.747301403011</v>
       </c>
-      <c r="M44" s="43">
+      <c r="M44" s="32">
         <f t="shared" si="1"/>
         <v>147629.71153724933</v>
       </c>
@@ -6626,7 +6614,7 @@
       <c r="A45" t="s">
         <v>152</v>
       </c>
-      <c r="B45" s="42">
+      <c r="B45" s="31">
         <v>21715</v>
       </c>
       <c r="C45">
@@ -6635,39 +6623,39 @@
       <c r="D45">
         <v>0.6</v>
       </c>
-      <c r="E45" s="43">
+      <c r="E45" s="32">
         <f t="shared" si="1"/>
         <v>9452.0027409876675</v>
       </c>
-      <c r="F45" s="43">
+      <c r="F45" s="32">
         <f t="shared" si="1"/>
         <v>14326.557141216699</v>
       </c>
-      <c r="G45" s="43">
+      <c r="G45" s="32">
         <f t="shared" si="1"/>
         <v>21715</v>
       </c>
-      <c r="H45" s="43">
+      <c r="H45" s="32">
         <f t="shared" si="1"/>
         <v>24825.948006504732</v>
       </c>
-      <c r="I45" s="43">
+      <c r="I45" s="32">
         <f t="shared" si="1"/>
         <v>27695.843031089047</v>
       </c>
-      <c r="J45" s="43">
+      <c r="J45" s="32">
         <f t="shared" si="1"/>
         <v>32913.785241773294</v>
       </c>
-      <c r="K45" s="43">
+      <c r="K45" s="32">
         <f t="shared" si="1"/>
         <v>49887.969557521232</v>
       </c>
-      <c r="L45" s="43">
+      <c r="L45" s="32">
         <f t="shared" si="1"/>
         <v>57035.051272627803</v>
       </c>
-      <c r="M45" s="43">
+      <c r="M45" s="32">
         <f t="shared" si="1"/>
         <v>86448.97208569193</v>
       </c>
@@ -6676,7 +6664,7 @@
       <c r="A46" t="s">
         <v>153</v>
       </c>
-      <c r="B46" s="42">
+      <c r="B46" s="31">
         <v>50244</v>
       </c>
       <c r="C46">
@@ -6685,39 +6673,39 @@
       <c r="D46">
         <v>0.7</v>
       </c>
-      <c r="E46" s="43">
+      <c r="E46" s="32">
         <f t="shared" si="1"/>
         <v>19038.915791937114</v>
       </c>
-      <c r="F46" s="43">
+      <c r="F46" s="32">
         <f t="shared" si="1"/>
         <v>30928.809952050986</v>
       </c>
-      <c r="G46" s="43">
+      <c r="G46" s="32">
         <f t="shared" si="1"/>
         <v>50244</v>
       </c>
-      <c r="H46" s="43">
+      <c r="H46" s="32">
         <f t="shared" si="1"/>
         <v>58738.27876549973</v>
       </c>
-      <c r="I46" s="43">
+      <c r="I46" s="32">
         <f t="shared" si="1"/>
         <v>66734.143099712877</v>
       </c>
-      <c r="J46" s="43">
+      <c r="J46" s="32">
         <f t="shared" si="1"/>
         <v>81621.618805045393</v>
       </c>
-      <c r="K46" s="43">
+      <c r="K46" s="32">
         <f t="shared" si="1"/>
         <v>132594.7109377466</v>
       </c>
-      <c r="L46" s="43">
+      <c r="L46" s="32">
         <f t="shared" si="1"/>
         <v>155011.24699252081</v>
       </c>
-      <c r="M46" s="43">
+      <c r="M46" s="32">
         <f t="shared" si="1"/>
         <v>251816.5136636867</v>
       </c>
@@ -6726,7 +6714,7 @@
       <c r="A47" t="s">
         <v>154</v>
       </c>
-      <c r="B47" s="42">
+      <c r="B47" s="31">
         <v>33067253</v>
       </c>
       <c r="C47">
@@ -6735,39 +6723,39 @@
       <c r="D47">
         <v>0.65</v>
       </c>
-      <c r="E47" s="43">
+      <c r="E47" s="32">
         <f t="shared" si="1"/>
         <v>13429477.745083958</v>
       </c>
-      <c r="F47" s="43">
+      <c r="F47" s="32">
         <f t="shared" si="1"/>
         <v>21073109.363702379</v>
       </c>
-      <c r="G47" s="43">
+      <c r="G47" s="32">
         <f t="shared" si="1"/>
         <v>33067253</v>
       </c>
-      <c r="H47" s="43">
+      <c r="H47" s="32">
         <f t="shared" si="1"/>
         <v>38228708.534664541</v>
       </c>
-      <c r="I47" s="43">
+      <c r="I47" s="32">
         <f t="shared" si="1"/>
         <v>43038530.714245498</v>
       </c>
-      <c r="J47" s="43">
+      <c r="J47" s="32">
         <f t="shared" si="1"/>
         <v>51888081.729857251</v>
       </c>
-      <c r="K47" s="43">
+      <c r="K47" s="32">
         <f t="shared" si="1"/>
         <v>81421127.591225848</v>
       </c>
-      <c r="L47" s="43">
+      <c r="L47" s="32">
         <f t="shared" si="1"/>
         <v>94130121.883686736</v>
       </c>
-      <c r="M47" s="43">
+      <c r="M47" s="32">
         <f t="shared" si="1"/>
         <v>147705993.52604714</v>
       </c>
@@ -6776,7 +6764,7 @@
       <c r="A48" t="s">
         <v>155</v>
       </c>
-      <c r="B48" s="42">
+      <c r="B48" s="31">
         <v>411911</v>
       </c>
       <c r="C48">
@@ -6785,39 +6773,39 @@
       <c r="D48">
         <v>0.65</v>
       </c>
-      <c r="E48" s="43">
+      <c r="E48" s="32">
         <f t="shared" si="1"/>
         <v>167287.84841774666</v>
       </c>
-      <c r="F48" s="43">
+      <c r="F48" s="32">
         <f t="shared" si="1"/>
         <v>262502.77127985231</v>
       </c>
-      <c r="G48" s="43">
+      <c r="G48" s="32">
         <f t="shared" si="1"/>
         <v>411911</v>
       </c>
-      <c r="H48" s="43">
+      <c r="H48" s="32">
         <f t="shared" si="1"/>
         <v>476206.03868190094</v>
       </c>
-      <c r="I48" s="43">
+      <c r="I48" s="32">
         <f t="shared" si="1"/>
         <v>536120.86329141329</v>
       </c>
-      <c r="J48" s="43">
+      <c r="J48" s="32">
         <f t="shared" si="1"/>
         <v>646357.64069749706</v>
       </c>
-      <c r="K48" s="43">
+      <c r="K48" s="32">
         <f t="shared" si="1"/>
         <v>1014243.8528906356</v>
       </c>
-      <c r="L48" s="43">
+      <c r="L48" s="32">
         <f t="shared" si="1"/>
         <v>1172556.808248671</v>
       </c>
-      <c r="M48" s="43">
+      <c r="M48" s="32">
         <f t="shared" si="1"/>
         <v>1839938.8512649538</v>
       </c>
@@ -6826,7 +6814,7 @@
       <c r="A49" t="s">
         <v>156</v>
       </c>
-      <c r="B49" s="42">
+      <c r="B49" s="31">
         <v>585966</v>
       </c>
       <c r="C49">
@@ -6835,39 +6823,39 @@
       <c r="D49">
         <v>0.65</v>
       </c>
-      <c r="E49" s="43">
+      <c r="E49" s="32">
         <f t="shared" si="1"/>
         <v>237976.14384163893</v>
       </c>
-      <c r="F49" s="43">
+      <c r="F49" s="32">
         <f t="shared" si="1"/>
         <v>373424.5962738794</v>
       </c>
-      <c r="G49" s="43">
+      <c r="G49" s="32">
         <f t="shared" si="1"/>
         <v>585966</v>
       </c>
-      <c r="H49" s="43">
+      <c r="H49" s="32">
         <f t="shared" si="1"/>
         <v>677429.22054103622</v>
       </c>
-      <c r="I49" s="43">
+      <c r="I49" s="32">
         <f t="shared" si="1"/>
         <v>762661.34621172119</v>
       </c>
-      <c r="J49" s="43">
+      <c r="J49" s="32">
         <f t="shared" si="1"/>
         <v>919479.21101633494</v>
       </c>
-      <c r="K49" s="43">
+      <c r="K49" s="32">
         <f t="shared" si="1"/>
         <v>1442817.5346201344</v>
       </c>
-      <c r="L49" s="43">
+      <c r="L49" s="32">
         <f t="shared" si="1"/>
         <v>1668026.4006113959</v>
       </c>
-      <c r="M49" s="43">
+      <c r="M49" s="32">
         <f t="shared" si="1"/>
         <v>2617413.9775833129</v>
       </c>
@@ -6876,7 +6864,7 @@
       <c r="A50" t="s">
         <v>157</v>
       </c>
-      <c r="B50" s="42">
+      <c r="B50" s="31">
         <v>326304</v>
       </c>
       <c r="C50">
@@ -6885,39 +6873,39 @@
       <c r="D50">
         <v>0.65</v>
       </c>
-      <c r="E50" s="43">
+      <c r="E50" s="32">
         <f t="shared" si="1"/>
         <v>132520.60297031252</v>
       </c>
-      <c r="F50" s="43">
+      <c r="F50" s="32">
         <f t="shared" si="1"/>
         <v>207947.11546839227</v>
       </c>
-      <c r="G50" s="43">
+      <c r="G50" s="32">
         <f t="shared" si="1"/>
         <v>326304</v>
       </c>
-      <c r="H50" s="43">
+      <c r="H50" s="32">
         <f t="shared" si="1"/>
         <v>377236.67308243527</v>
       </c>
-      <c r="I50" s="43">
+      <c r="I50" s="32">
         <f t="shared" si="1"/>
         <v>424699.46705827554</v>
       </c>
-      <c r="J50" s="43">
+      <c r="J50" s="32">
         <f t="shared" si="1"/>
         <v>512025.85896020272</v>
       </c>
-      <c r="K50" s="43">
+      <c r="K50" s="32">
         <f t="shared" si="1"/>
         <v>803454.69330419914</v>
       </c>
-      <c r="L50" s="43">
+      <c r="L50" s="32">
         <f t="shared" si="1"/>
         <v>928865.6451485256</v>
       </c>
-      <c r="M50" s="43">
+      <c r="M50" s="32">
         <f t="shared" si="1"/>
         <v>1457546.4285322789</v>
       </c>
@@ -6926,7 +6914,7 @@
       <c r="A51" t="s">
         <v>165</v>
       </c>
-      <c r="B51" s="42">
+      <c r="B51" s="31">
         <v>178050</v>
       </c>
       <c r="C51">
@@ -6935,39 +6923,39 @@
       <c r="D51">
         <v>0.65</v>
       </c>
-      <c r="E51" s="43">
+      <c r="E51" s="32">
         <f t="shared" si="1"/>
         <v>72310.76958561386</v>
       </c>
-      <c r="F51" s="43">
+      <c r="F51" s="32">
         <f t="shared" si="1"/>
         <v>113467.75984709732</v>
       </c>
-      <c r="G51" s="43">
+      <c r="G51" s="32">
         <f t="shared" si="1"/>
         <v>178050</v>
       </c>
-      <c r="H51" s="43">
+      <c r="H51" s="32">
         <f t="shared" si="1"/>
         <v>205841.75996104124</v>
       </c>
-      <c r="I51" s="43">
+      <c r="I51" s="32">
         <f t="shared" si="1"/>
         <v>231740.15675482361</v>
       </c>
-      <c r="J51" s="43">
+      <c r="J51" s="32">
         <f t="shared" si="1"/>
         <v>279390.39726103295</v>
       </c>
-      <c r="K51" s="43">
+      <c r="K51" s="32">
         <f t="shared" si="1"/>
         <v>438410.52559212467</v>
       </c>
-      <c r="L51" s="43">
+      <c r="L51" s="32">
         <f t="shared" si="1"/>
         <v>506841.86561824247</v>
       </c>
-      <c r="M51" s="43">
+      <c r="M51" s="32">
         <f t="shared" si="1"/>
         <v>795320.13582478999</v>
       </c>
@@ -6976,7 +6964,7 @@
       <c r="A52" t="s">
         <v>158</v>
       </c>
-      <c r="B52" s="42">
+      <c r="B52" s="31">
         <v>223100</v>
       </c>
       <c r="C52">
@@ -6985,39 +6973,39 @@
       <c r="D52">
         <v>0.7</v>
       </c>
-      <c r="E52" s="43">
+      <c r="E52" s="32">
         <f t="shared" si="1"/>
         <v>84539.091497117464</v>
       </c>
-      <c r="F52" s="43">
+      <c r="F52" s="32">
         <f t="shared" si="1"/>
         <v>137334.15930862541</v>
       </c>
-      <c r="G52" s="43">
+      <c r="G52" s="32">
         <f t="shared" si="1"/>
         <v>223100</v>
       </c>
-      <c r="H52" s="43">
+      <c r="H52" s="32">
         <f t="shared" si="1"/>
         <v>260817.4108865335</v>
       </c>
-      <c r="I52" s="43">
+      <c r="I52" s="32">
         <f t="shared" si="1"/>
         <v>296321.69663135783</v>
       </c>
-      <c r="J52" s="43">
+      <c r="J52" s="32">
         <f t="shared" si="1"/>
         <v>362427.01925415226</v>
       </c>
-      <c r="K52" s="43">
+      <c r="K52" s="32">
         <f t="shared" si="1"/>
         <v>588764.42978686537</v>
       </c>
-      <c r="L52" s="43">
+      <c r="L52" s="32">
         <f t="shared" si="1"/>
         <v>688301.27386417065</v>
       </c>
-      <c r="M52" s="43">
+      <c r="M52" s="32">
         <f t="shared" si="1"/>
         <v>1118148.7182224444</v>
       </c>
@@ -7026,7 +7014,7 @@
       <c r="A53" t="s">
         <v>159</v>
       </c>
-      <c r="B53" s="42">
+      <c r="B53" s="31">
         <v>27883640</v>
       </c>
       <c r="C53">
@@ -7035,39 +7023,39 @@
       <c r="D53">
         <v>0.6</v>
       </c>
-      <c r="E53" s="43">
+      <c r="E53" s="32">
         <f t="shared" si="1"/>
         <v>12137059.254373169</v>
       </c>
-      <c r="F53" s="43">
+      <c r="F53" s="32">
         <f t="shared" si="1"/>
         <v>18396341.780571751</v>
       </c>
-      <c r="G53" s="43">
+      <c r="G53" s="32">
         <f t="shared" si="1"/>
         <v>27883640</v>
       </c>
-      <c r="H53" s="43">
+      <c r="H53" s="32">
         <f t="shared" si="1"/>
         <v>31878323.595307186</v>
       </c>
-      <c r="I53" s="43">
+      <c r="I53" s="32">
         <f t="shared" si="1"/>
         <v>35563477.622629322</v>
       </c>
-      <c r="J53" s="43">
+      <c r="J53" s="32">
         <f t="shared" si="1"/>
         <v>42263695.082611993</v>
       </c>
-      <c r="K53" s="43">
+      <c r="K53" s="32">
         <f t="shared" si="1"/>
         <v>64059782.798659056</v>
       </c>
-      <c r="L53" s="43">
+      <c r="L53" s="32">
         <f t="shared" si="1"/>
         <v>73237155.74798505</v>
       </c>
-      <c r="M53" s="43">
+      <c r="M53" s="32">
         <f t="shared" si="1"/>
         <v>111006770.25132319</v>
       </c>
@@ -7076,7 +7064,7 @@
       <c r="A54" t="s">
         <v>160</v>
       </c>
-      <c r="B54" s="42">
+      <c r="B54" s="31">
         <v>11065762</v>
       </c>
       <c r="C54">
@@ -7085,39 +7073,39 @@
       <c r="D54">
         <v>0.6</v>
       </c>
-      <c r="E54" s="43">
+      <c r="E54" s="32">
         <f t="shared" si="1"/>
         <v>4816652.6712004226</v>
       </c>
-      <c r="F54" s="43">
+      <c r="F54" s="32">
         <f t="shared" si="1"/>
         <v>7300680.2488650419</v>
       </c>
-      <c r="G54" s="43">
+      <c r="G54" s="32">
         <f t="shared" si="1"/>
         <v>11065762</v>
       </c>
-      <c r="H54" s="43">
+      <c r="H54" s="32">
         <f t="shared" si="1"/>
         <v>12651072.165063588</v>
       </c>
-      <c r="I54" s="43">
+      <c r="I54" s="32">
         <f t="shared" si="1"/>
         <v>14113543.972893851</v>
       </c>
-      <c r="J54" s="43">
+      <c r="J54" s="32">
         <f t="shared" si="1"/>
         <v>16772558.784461234</v>
       </c>
-      <c r="K54" s="43">
+      <c r="K54" s="32">
         <f t="shared" si="1"/>
         <v>25422445.212377403</v>
       </c>
-      <c r="L54" s="43">
+      <c r="L54" s="32">
         <f t="shared" si="1"/>
         <v>29064531.569914639</v>
       </c>
-      <c r="M54" s="43">
+      <c r="M54" s="32">
         <f t="shared" si="1"/>
         <v>44053591.998384088</v>
       </c>
@@ -7126,7 +7114,7 @@
       <c r="A55" t="s">
         <v>161</v>
       </c>
-      <c r="B55" s="42">
+      <c r="B55" s="31">
         <v>6015366</v>
       </c>
       <c r="C55">
@@ -7135,39 +7123,39 @@
       <c r="D55">
         <v>0.6</v>
       </c>
-      <c r="E55" s="43">
+      <c r="E55" s="32">
         <f t="shared" si="1"/>
         <v>2618340.1298661763</v>
       </c>
-      <c r="F55" s="43">
+      <c r="F55" s="32">
         <f t="shared" si="1"/>
         <v>3968661.5115971509</v>
       </c>
-      <c r="G55" s="43">
+      <c r="G55" s="32">
         <f t="shared" si="1"/>
         <v>6015366</v>
       </c>
-      <c r="H55" s="43">
+      <c r="H55" s="32">
         <f t="shared" si="1"/>
         <v>6877143.152479684</v>
       </c>
-      <c r="I55" s="43">
+      <c r="I55" s="32">
         <f t="shared" si="1"/>
         <v>7672145.1766313603</v>
       </c>
-      <c r="J55" s="43">
+      <c r="J55" s="32">
         <f t="shared" si="1"/>
         <v>9117589.8998233862</v>
       </c>
-      <c r="K55" s="43">
+      <c r="K55" s="32">
         <f t="shared" si="1"/>
         <v>13819682.057810189</v>
       </c>
-      <c r="L55" s="43">
+      <c r="L55" s="32">
         <f t="shared" si="1"/>
         <v>15799526.05266507</v>
       </c>
-      <c r="M55" s="43">
+      <c r="M55" s="32">
         <f t="shared" si="1"/>
         <v>23947603.381037086</v>
       </c>
@@ -7176,7 +7164,7 @@
       <c r="A56" t="s">
         <v>164</v>
       </c>
-      <c r="B56" s="42">
+      <c r="B56" s="31">
         <v>1779507</v>
       </c>
       <c r="C56">
@@ -7185,39 +7173,39 @@
       <c r="D56">
         <v>0.6</v>
       </c>
-      <c r="E56" s="43">
+      <c r="E56" s="32">
         <f t="shared" si="1"/>
         <v>774575.410619698</v>
       </c>
-      <c r="F56" s="43">
+      <c r="F56" s="32">
         <f t="shared" si="1"/>
         <v>1174036.7818878703</v>
       </c>
-      <c r="G56" s="43">
+      <c r="G56" s="32">
         <f t="shared" si="1"/>
         <v>1779507</v>
       </c>
-      <c r="H56" s="43">
+      <c r="H56" s="32">
         <f t="shared" si="1"/>
         <v>2034443.8526001018</v>
       </c>
-      <c r="I56" s="43">
+      <c r="I56" s="32">
         <f t="shared" si="1"/>
         <v>2269626.8268350991</v>
       </c>
-      <c r="J56" s="43">
+      <c r="J56" s="32">
         <f t="shared" si="1"/>
         <v>2697228.2401212188</v>
       </c>
-      <c r="K56" s="43">
+      <c r="K56" s="32">
         <f t="shared" si="1"/>
         <v>4088233.5272114179</v>
       </c>
-      <c r="L56" s="43">
+      <c r="L56" s="32">
         <f t="shared" si="1"/>
         <v>4673924.6136311339</v>
       </c>
-      <c r="M56" s="43">
+      <c r="M56" s="32">
         <f t="shared" si="1"/>
         <v>7084344.9675014224</v>
       </c>
@@ -7226,7 +7214,7 @@
       <c r="A57" t="s">
         <v>162</v>
       </c>
-      <c r="B57" s="42">
+      <c r="B57" s="31">
         <v>2929758</v>
       </c>
       <c r="C57">
@@ -7235,39 +7223,39 @@
       <c r="D57">
         <v>0.6</v>
       </c>
-      <c r="E57" s="43">
+      <c r="E57" s="32">
         <f t="shared" si="1"/>
         <v>1275251.238610663</v>
       </c>
-      <c r="F57" s="43">
+      <c r="F57" s="32">
         <f t="shared" si="1"/>
         <v>1932919.4288250864</v>
       </c>
-      <c r="G57" s="43">
+      <c r="G57" s="32">
         <f t="shared" si="1"/>
         <v>2929758</v>
       </c>
-      <c r="H57" s="43">
+      <c r="H57" s="32">
         <f t="shared" si="1"/>
         <v>3349482.8358112499</v>
       </c>
-      <c r="I57" s="43">
+      <c r="I57" s="32">
         <f t="shared" si="1"/>
         <v>3736685.1341044153</v>
       </c>
-      <c r="J57" s="43">
+      <c r="J57" s="32">
         <f t="shared" si="1"/>
         <v>4440682.7364663705</v>
       </c>
-      <c r="K57" s="43">
+      <c r="K57" s="32">
         <f t="shared" si="1"/>
         <v>6730816.3902788069</v>
       </c>
-      <c r="L57" s="43">
+      <c r="L57" s="32">
         <f t="shared" si="1"/>
         <v>7695090.8471743716</v>
       </c>
-      <c r="M57" s="43">
+      <c r="M57" s="32">
         <f t="shared" si="1"/>
         <v>11663576.67786473</v>
       </c>
@@ -7276,7 +7264,7 @@
       <c r="A58" t="s">
         <v>163</v>
       </c>
-      <c r="B58" s="42">
+      <c r="B58" s="31">
         <v>7405996</v>
       </c>
       <c r="C58">
@@ -7285,39 +7273,39 @@
       <c r="D58">
         <v>0.65</v>
       </c>
-      <c r="E58" s="43">
+      <c r="E58" s="32">
         <f t="shared" si="1"/>
         <v>3007768.9992023474</v>
       </c>
-      <c r="F58" s="43">
+      <c r="F58" s="32">
         <f t="shared" si="1"/>
         <v>4719695.4538419731</v>
       </c>
-      <c r="G58" s="43">
+      <c r="G58" s="32">
         <f t="shared" si="1"/>
         <v>7405996</v>
       </c>
-      <c r="H58" s="43">
+      <c r="H58" s="32">
         <f t="shared" si="1"/>
         <v>8561995.2311397456</v>
       </c>
-      <c r="I58" s="43">
+      <c r="I58" s="32">
         <f t="shared" si="1"/>
         <v>9639239.9548755772</v>
       </c>
-      <c r="J58" s="43">
+      <c r="J58" s="32">
         <f t="shared" si="1"/>
         <v>11621253.38137389</v>
       </c>
-      <c r="K58" s="43">
+      <c r="K58" s="32">
         <f t="shared" si="1"/>
         <v>18235701.201309595</v>
       </c>
-      <c r="L58" s="43">
+      <c r="L58" s="32">
         <f t="shared" si="1"/>
         <v>21082105.191807028</v>
       </c>
-      <c r="M58" s="43">
+      <c r="M58" s="32">
         <f t="shared" si="1"/>
         <v>33081368.967356648</v>
       </c>
@@ -7326,39 +7314,39 @@
       <c r="D60" t="s">
         <v>166</v>
       </c>
-      <c r="E60" s="44">
+      <c r="E60">
         <f>E24</f>
         <v>0.25</v>
       </c>
-      <c r="F60" s="44">
+      <c r="F60">
         <f t="shared" ref="F60:M60" si="2">F24</f>
         <v>0.5</v>
       </c>
-      <c r="G60" s="44">
+      <c r="G60">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="H60" s="44">
+      <c r="H60">
         <f t="shared" si="2"/>
         <v>1.25</v>
       </c>
-      <c r="I60" s="44">
+      <c r="I60">
         <f t="shared" si="2"/>
         <v>1.5</v>
       </c>
-      <c r="J60" s="44">
+      <c r="J60">
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
-      <c r="K60" s="44">
+      <c r="K60">
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
-      <c r="L60" s="44">
+      <c r="L60">
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
-      <c r="M60" s="44">
+      <c r="M60">
         <f t="shared" si="2"/>
         <v>10</v>
       </c>
@@ -7367,39 +7355,39 @@
       <c r="D61" t="s">
         <v>112</v>
       </c>
-      <c r="E61" s="43">
+      <c r="E61" s="32">
         <f>SUM(E25:E58)</f>
         <v>103661944.99376373</v>
       </c>
-      <c r="F61" s="43">
+      <c r="F61" s="32">
         <f t="shared" ref="F61:M61" si="3">SUM(F25:F58)</f>
         <v>163252732.89508671</v>
       </c>
-      <c r="G61" s="43">
+      <c r="G61" s="32">
         <f>SUM(G25:G58)</f>
         <v>257800646</v>
       </c>
-      <c r="H61" s="43">
+      <c r="H61" s="32">
         <f t="shared" si="3"/>
         <v>298830505.00587934</v>
       </c>
-      <c r="I61" s="43">
+      <c r="I61" s="32">
         <f t="shared" si="3"/>
         <v>337232658.66429305</v>
       </c>
-      <c r="J61" s="43">
+      <c r="J61" s="32">
         <f t="shared" si="3"/>
         <v>408279669.36056608</v>
       </c>
-      <c r="K61" s="43">
+      <c r="K61" s="32">
         <f t="shared" si="3"/>
         <v>648555689.20624173</v>
       </c>
-      <c r="L61" s="43">
+      <c r="L61" s="32">
         <f t="shared" si="3"/>
         <v>753254554.49843431</v>
       </c>
-      <c r="M61" s="43">
+      <c r="M61" s="32">
         <f t="shared" si="3"/>
         <v>1201614609.967025</v>
       </c>
@@ -7408,39 +7396,39 @@
       <c r="D62" t="s">
         <v>168</v>
       </c>
-      <c r="E62" s="44">
+      <c r="E62">
         <f>LOG(E60)</f>
         <v>-0.6020599913279624</v>
       </c>
-      <c r="F62" s="44">
+      <c r="F62">
         <f t="shared" ref="F62:M62" si="4">LOG(F60)</f>
         <v>-0.3010299956639812</v>
       </c>
-      <c r="G62" s="44">
+      <c r="G62">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="H62" s="44">
+      <c r="H62">
         <f t="shared" si="4"/>
         <v>9.691001300805642E-2</v>
       </c>
-      <c r="I62" s="44">
+      <c r="I62">
         <f t="shared" si="4"/>
         <v>0.17609125905568124</v>
       </c>
-      <c r="J62" s="44">
+      <c r="J62">
         <f t="shared" si="4"/>
         <v>0.3010299956639812</v>
       </c>
-      <c r="K62" s="44">
+      <c r="K62">
         <f t="shared" si="4"/>
         <v>0.6020599913279624</v>
       </c>
-      <c r="L62" s="44">
+      <c r="L62">
         <f t="shared" si="4"/>
         <v>0.69897000433601886</v>
       </c>
-      <c r="M62" s="44">
+      <c r="M62">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
@@ -7494,7 +7482,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E40FBC7-515F-444A-AA65-63C61A66544C}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="F6" sqref="F6"/>
@@ -7508,101 +7496,100 @@
     <col min="4" max="4" width="10.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="50" t="s">
+    <row r="1" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
         <v>220</v>
       </c>
-      <c r="B1" s="57" t="s">
+      <c r="B1" s="44" t="s">
         <v>219</v>
       </c>
-      <c r="C1" s="57"/>
-      <c r="D1" s="57"/>
-      <c r="E1" s="57"/>
-      <c r="F1" s="50"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="51" t="s">
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="37" t="s">
         <v>84</v>
       </c>
-      <c r="B2" s="52">
+      <c r="B2" s="38">
         <v>50</v>
       </c>
-      <c r="C2" s="52">
+      <c r="C2" s="38">
         <v>300</v>
       </c>
-      <c r="D2" s="53">
+      <c r="D2" s="39">
         <v>1000</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="22" t="s">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="12">
+      <c r="B3">
         <f>-B2-$B4</f>
         <v>-35.1</v>
       </c>
-      <c r="C3" s="12">
+      <c r="C3">
         <f t="shared" ref="C3:D3" si="0">-C2-$B4</f>
         <v>-285.10000000000002</v>
       </c>
-      <c r="D3" s="23">
+      <c r="D3" s="20">
         <f t="shared" si="0"/>
         <v>-985.1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="22" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="19" t="s">
         <v>169</v>
       </c>
-      <c r="B4" s="58">
+      <c r="B4" s="44">
         <v>-14.9</v>
       </c>
-      <c r="C4" s="58"/>
-      <c r="D4" s="59"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="22" t="s">
+      <c r="C4" s="44"/>
+      <c r="D4" s="45"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="19" t="s">
         <v>170</v>
       </c>
-      <c r="B5" s="12">
+      <c r="B5">
         <v>25.13</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" t="s">
         <v>171</v>
       </c>
-      <c r="D5" s="23"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="22" t="s">
+      <c r="D5" s="20"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="19" t="s">
         <v>172</v>
       </c>
-      <c r="B6" s="12">
+      <c r="B6">
         <f>ABS(B3)*$B5</f>
         <v>882.06299999999999</v>
       </c>
-      <c r="C6" s="12">
+      <c r="C6">
         <f t="shared" ref="C6:D6" si="1">ABS(C3)*$B5</f>
         <v>7164.5630000000001</v>
       </c>
-      <c r="D6" s="23">
+      <c r="D6" s="20">
         <f t="shared" si="1"/>
         <v>24755.562999999998</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="40" t="s">
+    <row r="7" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="23" t="s">
         <v>173</v>
       </c>
-      <c r="B7" s="31">
+      <c r="B7" s="24">
         <f>-B6</f>
         <v>-882.06299999999999</v>
       </c>
-      <c r="C7" s="31">
+      <c r="C7" s="24">
         <f t="shared" ref="C7:D7" si="2">-C6</f>
         <v>-7164.5630000000001</v>
       </c>
-      <c r="D7" s="41">
+      <c r="D7" s="26">
         <f t="shared" si="2"/>
         <v>-24755.562999999998</v>
       </c>
@@ -7823,7 +7810,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75BB7584-3066-8D4D-9480-F9C4BB723ACA}">
   <dimension ref="A1:H31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
@@ -7874,446 +7861,432 @@
       <c r="A6" t="s">
         <v>175</v>
       </c>
-      <c r="B6" s="60" t="s">
+      <c r="B6" s="46" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="61"/>
-      <c r="D6" s="61"/>
-      <c r="E6" s="61"/>
-      <c r="F6" s="61"/>
-      <c r="G6" s="61"/>
-      <c r="H6" s="62"/>
+      <c r="C6" s="47"/>
+      <c r="D6" s="47"/>
+      <c r="E6" s="47"/>
+      <c r="F6" s="47"/>
+      <c r="G6" s="47"/>
+      <c r="H6" s="48"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B7" s="22" t="s">
+      <c r="B7" s="19" t="s">
         <v>179</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="C7" t="s">
         <v>180</v>
       </c>
-      <c r="D7" s="12" t="s">
+      <c r="D7" t="s">
         <v>27</v>
       </c>
-      <c r="E7" s="12" t="s">
+      <c r="E7" t="s">
         <v>28</v>
       </c>
-      <c r="F7" s="12" t="s">
+      <c r="F7" t="s">
         <v>48</v>
       </c>
-      <c r="G7" s="12" t="s">
+      <c r="G7" t="s">
         <v>181</v>
       </c>
-      <c r="H7" s="23"/>
+      <c r="H7" s="20"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B8" s="22" t="s">
+      <c r="B8" s="19" t="s">
         <v>182</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="C8" t="s">
         <v>183</v>
       </c>
-      <c r="D8" s="12">
+      <c r="D8">
         <v>1</v>
       </c>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12" t="s">
+      <c r="F8" t="s">
         <v>184</v>
       </c>
-      <c r="G8" s="12" t="s">
+      <c r="G8" t="s">
         <v>34</v>
       </c>
-      <c r="H8" s="23"/>
+      <c r="H8" s="20"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B9" s="22" t="s">
+      <c r="B9" s="19" t="s">
         <v>201</v>
       </c>
-      <c r="C9" s="12"/>
-      <c r="D9" s="12">
+      <c r="D9">
         <v>20</v>
       </c>
-      <c r="E9" s="12" t="s">
+      <c r="E9" t="s">
         <v>39</v>
       </c>
-      <c r="F9" s="12"/>
-      <c r="G9" s="12"/>
-      <c r="H9" s="23"/>
+      <c r="H9" s="20"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B10" s="22" t="s">
+      <c r="B10" s="19" t="s">
         <v>185</v>
       </c>
-      <c r="C10" s="12" t="s">
+      <c r="C10" t="s">
         <v>186</v>
       </c>
-      <c r="D10" s="12">
+      <c r="D10">
         <v>-30320</v>
       </c>
-      <c r="E10" s="12" t="s">
+      <c r="E10" t="s">
         <v>187</v>
       </c>
-      <c r="F10" s="12" t="s">
+      <c r="F10" t="s">
         <v>188</v>
       </c>
-      <c r="G10" s="12" t="s">
+      <c r="G10" t="s">
         <v>189</v>
       </c>
-      <c r="H10" s="23"/>
+      <c r="H10" s="20"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B11" s="22" t="s">
+      <c r="B11" s="19" t="s">
         <v>190</v>
       </c>
-      <c r="C11" s="12" t="s">
+      <c r="C11" t="s">
         <v>191</v>
       </c>
-      <c r="D11" s="12">
+      <c r="D11">
         <v>-3.1680000000000001</v>
       </c>
-      <c r="E11" s="12" t="s">
+      <c r="E11" t="s">
         <v>192</v>
       </c>
-      <c r="F11" s="12" t="s">
+      <c r="F11" t="s">
         <v>193</v>
       </c>
-      <c r="G11" s="12" t="s">
+      <c r="G11" t="s">
         <v>189</v>
       </c>
-      <c r="H11" s="23"/>
+      <c r="H11" s="20"/>
     </row>
     <row r="12" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="40" t="s">
+      <c r="B12" s="23" t="s">
         <v>194</v>
       </c>
-      <c r="C12" s="31" t="s">
+      <c r="C12" s="24" t="s">
         <v>186</v>
       </c>
-      <c r="D12" s="31">
+      <c r="D12" s="24">
         <v>-27933.45</v>
       </c>
-      <c r="E12" s="31" t="s">
+      <c r="E12" s="24" t="s">
         <v>195</v>
       </c>
-      <c r="F12" s="31" t="s">
+      <c r="F12" s="24" t="s">
         <v>188</v>
       </c>
-      <c r="G12" s="31" t="s">
+      <c r="G12" s="24" t="s">
         <v>189</v>
       </c>
-      <c r="H12" s="41"/>
+      <c r="H12" s="26"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B13" s="60" t="s">
+      <c r="B13" s="46" t="s">
         <v>285</v>
       </c>
-      <c r="C13" s="61"/>
-      <c r="D13" s="61"/>
-      <c r="E13" s="61"/>
-      <c r="F13" s="61"/>
-      <c r="G13" s="61"/>
-      <c r="H13" s="62"/>
+      <c r="C13" s="47"/>
+      <c r="D13" s="47"/>
+      <c r="E13" s="47"/>
+      <c r="F13" s="47"/>
+      <c r="G13" s="47"/>
+      <c r="H13" s="48"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B14" s="22" t="s">
+      <c r="B14" s="19" t="s">
         <v>179</v>
       </c>
-      <c r="C14" s="12" t="s">
+      <c r="C14" t="s">
         <v>180</v>
       </c>
-      <c r="D14" s="12" t="s">
+      <c r="D14" t="s">
         <v>27</v>
       </c>
-      <c r="E14" s="12" t="s">
+      <c r="E14" t="s">
         <v>28</v>
       </c>
-      <c r="F14" s="12" t="s">
+      <c r="F14" t="s">
         <v>48</v>
       </c>
-      <c r="G14" s="12" t="s">
+      <c r="G14" t="s">
         <v>181</v>
       </c>
-      <c r="H14" s="23"/>
+      <c r="H14" s="20"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B15" s="22" t="s">
+      <c r="B15" s="19" t="s">
         <v>196</v>
       </c>
-      <c r="C15" s="12" t="s">
+      <c r="C15" t="s">
         <v>286</v>
       </c>
-      <c r="D15" s="12"/>
-      <c r="E15" s="47"/>
-      <c r="F15" s="12"/>
-      <c r="G15" s="12"/>
-      <c r="H15" s="23"/>
+      <c r="E15" s="35"/>
+      <c r="H15" s="20"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B16" s="22"/>
-      <c r="C16" s="49" t="s">
+      <c r="B16" s="19"/>
+      <c r="C16" t="s">
         <v>288</v>
       </c>
-      <c r="D16" s="49">
+      <c r="D16">
         <v>400</v>
       </c>
-      <c r="E16" s="47" t="s">
+      <c r="E16" s="35" t="s">
         <v>289</v>
       </c>
-      <c r="F16" s="12"/>
-      <c r="G16" s="12"/>
-      <c r="H16" s="23"/>
+      <c r="H16" s="20"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B17" s="22"/>
-      <c r="C17" s="49" t="s">
+      <c r="B17" s="19"/>
+      <c r="C17" t="s">
         <v>290</v>
       </c>
-      <c r="D17" s="12">
+      <c r="D17">
         <f>-FT!B15</f>
         <v>-158102945</v>
       </c>
-      <c r="E17" s="63" t="s">
+      <c r="E17" s="1" t="s">
         <v>283</v>
       </c>
-      <c r="F17" s="49" t="s">
+      <c r="F17" t="s">
         <v>184</v>
       </c>
-      <c r="G17" s="49" t="s">
+      <c r="G17" t="s">
         <v>200</v>
       </c>
-      <c r="H17" s="23"/>
+      <c r="H17" s="20"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B18" s="22"/>
-      <c r="C18" s="49" t="s">
+      <c r="B18" s="19"/>
+      <c r="C18" t="s">
         <v>287</v>
       </c>
-      <c r="D18" s="49">
+      <c r="D18">
         <v>0.626</v>
       </c>
-      <c r="E18" s="47"/>
-      <c r="F18" s="12"/>
-      <c r="G18" s="12"/>
-      <c r="H18" s="23"/>
+      <c r="E18" s="35"/>
+      <c r="H18" s="20"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B19" s="22" t="s">
+      <c r="B19" s="19" t="s">
         <v>201</v>
       </c>
-      <c r="C19" s="12"/>
-      <c r="D19" s="12">
+      <c r="D19">
         <v>20</v>
       </c>
-      <c r="E19" s="12" t="s">
+      <c r="E19" t="s">
         <v>39</v>
       </c>
-      <c r="F19" s="12"/>
-      <c r="G19" s="12"/>
-      <c r="H19" s="23"/>
+      <c r="H19" s="20"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B20" s="22" t="s">
+      <c r="B20" s="19" t="s">
         <v>202</v>
       </c>
-      <c r="C20" s="12">
+      <c r="C20">
         <v>1</v>
       </c>
-      <c r="D20" s="64">
+      <c r="D20" s="43">
         <v>-21732221</v>
       </c>
-      <c r="E20" s="12" t="s">
+      <c r="E20" t="s">
         <v>203</v>
       </c>
-      <c r="F20" s="12" t="s">
+      <c r="F20" t="s">
         <v>188</v>
       </c>
-      <c r="G20" s="12" t="s">
+      <c r="G20" t="s">
         <v>189</v>
       </c>
-      <c r="H20" s="23"/>
+      <c r="H20" s="20"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B21" s="22" t="s">
+      <c r="B21" s="19" t="s">
         <v>204</v>
       </c>
-      <c r="C21" s="12">
+      <c r="C21">
         <v>1</v>
       </c>
-      <c r="D21" s="12">
+      <c r="D21">
         <v>-9636868</v>
       </c>
-      <c r="E21" s="12" t="s">
+      <c r="E21" t="s">
         <v>203</v>
       </c>
-      <c r="F21" s="12" t="s">
+      <c r="F21" t="s">
         <v>188</v>
       </c>
-      <c r="G21" s="12" t="s">
+      <c r="G21" t="s">
         <v>189</v>
       </c>
-      <c r="H21" s="23"/>
+      <c r="H21" s="20"/>
     </row>
     <row r="22" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="48" t="s">
+      <c r="B22" s="36" t="s">
         <v>207</v>
       </c>
-      <c r="C22" s="31" t="s">
+      <c r="C22" s="24" t="s">
         <v>205</v>
       </c>
-      <c r="D22" s="31">
+      <c r="D22" s="24">
         <v>0.13100999999999999</v>
       </c>
-      <c r="E22" s="31" t="s">
+      <c r="E22" s="24" t="s">
         <v>206</v>
       </c>
-      <c r="F22" s="31" t="s">
+      <c r="F22" s="24" t="s">
         <v>193</v>
       </c>
-      <c r="G22" s="31" t="s">
+      <c r="G22" s="24" t="s">
         <v>189</v>
       </c>
-      <c r="H22" s="41"/>
+      <c r="H22" s="26"/>
     </row>
     <row r="23" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A24" s="60" t="s">
+      <c r="A24" s="46" t="s">
         <v>209</v>
       </c>
-      <c r="B24" s="61"/>
-      <c r="C24" s="61"/>
-      <c r="D24" s="62"/>
-      <c r="G24" s="60" t="s">
+      <c r="B24" s="47"/>
+      <c r="C24" s="47"/>
+      <c r="D24" s="48"/>
+      <c r="G24" s="46" t="s">
         <v>214</v>
       </c>
-      <c r="H24" s="62"/>
+      <c r="H24" s="48"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A25" s="22" t="s">
+      <c r="A25" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="B25" s="12" t="s">
+      <c r="B25" t="s">
         <v>210</v>
       </c>
-      <c r="C25" s="12" t="s">
+      <c r="C25" t="s">
         <v>208</v>
       </c>
-      <c r="D25" s="23" t="s">
+      <c r="D25" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="G25" s="22" t="s">
+      <c r="G25" s="19" t="s">
         <v>210</v>
       </c>
-      <c r="H25" s="23" t="s">
+      <c r="H25" s="20" t="s">
         <v>208</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A26" s="22" t="s">
+      <c r="A26" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="B26" s="12" t="s">
+      <c r="B26" t="s">
         <v>174</v>
       </c>
-      <c r="C26" s="12">
+      <c r="C26">
         <v>-1</v>
       </c>
-      <c r="D26" s="23" t="s">
+      <c r="D26" s="20" t="s">
         <v>215</v>
       </c>
-      <c r="G26" s="22" t="s">
+      <c r="G26" s="19" t="s">
         <v>174</v>
       </c>
-      <c r="H26" s="45">
+      <c r="H26" s="33">
         <v>-1</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A27" s="22" t="s">
+      <c r="A27" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="B27" s="12" t="s">
+      <c r="B27" t="s">
         <v>205</v>
       </c>
-      <c r="C27" s="12">
+      <c r="C27">
         <v>25.13</v>
       </c>
-      <c r="D27" s="23" t="s">
+      <c r="D27" s="20" t="s">
         <v>216</v>
       </c>
-      <c r="G27" s="22" t="s">
+      <c r="G27" s="19" t="s">
         <v>211</v>
       </c>
-      <c r="H27" s="45">
+      <c r="H27" s="33">
         <f>(C29/ABS(C$28))*(C$27)</f>
         <v>17.377632075471695</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A28" s="22" t="s">
+      <c r="A28" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="B28" s="12" t="s">
+      <c r="B28" t="s">
         <v>205</v>
       </c>
-      <c r="C28" s="12">
+      <c r="C28">
         <v>-1.06</v>
       </c>
-      <c r="D28" s="23" t="s">
+      <c r="D28" s="20" t="s">
         <v>216</v>
       </c>
-      <c r="G28" s="22" t="s">
+      <c r="G28" s="19" t="s">
         <v>212</v>
       </c>
-      <c r="H28" s="45">
+      <c r="H28" s="33">
         <f>(C30/ABS(C$28))*(C$27)</f>
         <v>21.052301886792449</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="22" t="s">
+      <c r="A29" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="B29" s="12" t="s">
+      <c r="B29" t="s">
         <v>211</v>
       </c>
-      <c r="C29" s="12">
+      <c r="C29">
         <v>0.73299999999999998</v>
       </c>
-      <c r="D29" s="23" t="s">
+      <c r="D29" s="20" t="s">
         <v>216</v>
       </c>
-      <c r="G29" s="40" t="s">
+      <c r="G29" s="23" t="s">
         <v>213</v>
       </c>
-      <c r="H29" s="46">
+      <c r="H29" s="34">
         <f>(C31/ABS(C$28))*(C$27)</f>
         <v>11.664113207547167</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A30" s="22" t="s">
+      <c r="A30" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="B30" s="12" t="s">
+      <c r="B30" t="s">
         <v>212</v>
       </c>
-      <c r="C30" s="12">
+      <c r="C30">
         <v>0.88800000000000001</v>
       </c>
-      <c r="D30" s="23" t="s">
+      <c r="D30" s="20" t="s">
         <v>216</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="40" t="s">
+      <c r="A31" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="B31" s="31" t="s">
+      <c r="B31" s="24" t="s">
         <v>213</v>
       </c>
-      <c r="C31" s="31">
+      <c r="C31" s="24">
         <v>0.49199999999999999</v>
       </c>
-      <c r="D31" s="41" t="s">
+      <c r="D31" s="26" t="s">
         <v>216</v>
       </c>
     </row>
@@ -8374,413 +8347,406 @@
       <c r="A5" t="s">
         <v>175</v>
       </c>
-      <c r="B5" s="60" t="s">
+      <c r="B5" s="46" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="61"/>
-      <c r="D5" s="61"/>
-      <c r="E5" s="61"/>
-      <c r="F5" s="61"/>
-      <c r="G5" s="61"/>
-      <c r="H5" s="62"/>
+      <c r="C5" s="47"/>
+      <c r="D5" s="47"/>
+      <c r="E5" s="47"/>
+      <c r="F5" s="47"/>
+      <c r="G5" s="47"/>
+      <c r="H5" s="48"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B6" s="22" t="s">
+      <c r="B6" s="19" t="s">
         <v>179</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C6" t="s">
         <v>180</v>
       </c>
-      <c r="D6" s="12" t="s">
+      <c r="D6" t="s">
         <v>27</v>
       </c>
-      <c r="E6" s="12" t="s">
+      <c r="E6" t="s">
         <v>28</v>
       </c>
-      <c r="F6" s="12" t="s">
+      <c r="F6" t="s">
         <v>48</v>
       </c>
-      <c r="G6" s="12" t="s">
+      <c r="G6" t="s">
         <v>181</v>
       </c>
-      <c r="H6" s="23"/>
+      <c r="H6" s="20"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B7" s="22" t="s">
+      <c r="B7" s="19" t="s">
         <v>182</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="C7" t="s">
         <v>183</v>
       </c>
-      <c r="D7" s="12">
+      <c r="D7">
         <v>1</v>
       </c>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12" t="s">
+      <c r="F7" t="s">
         <v>184</v>
       </c>
-      <c r="G7" s="12" t="s">
+      <c r="G7" t="s">
         <v>34</v>
       </c>
-      <c r="H7" s="23"/>
+      <c r="H7" s="20"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B8" s="22" t="s">
+      <c r="B8" s="19" t="s">
         <v>201</v>
       </c>
-      <c r="C8" s="12"/>
-      <c r="D8" s="12">
+      <c r="D8">
         <v>20</v>
       </c>
-      <c r="E8" s="12" t="s">
+      <c r="E8" t="s">
         <v>39</v>
       </c>
-      <c r="F8" s="12"/>
-      <c r="G8" s="12"/>
-      <c r="H8" s="23"/>
+      <c r="H8" s="20"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B9" s="22" t="s">
+      <c r="B9" s="19" t="s">
         <v>185</v>
       </c>
-      <c r="C9" s="12" t="s">
+      <c r="C9" t="s">
         <v>186</v>
       </c>
-      <c r="D9" s="12">
+      <c r="D9">
         <v>-30320</v>
       </c>
-      <c r="E9" s="12" t="s">
+      <c r="E9" t="s">
         <v>187</v>
       </c>
-      <c r="F9" s="12" t="s">
+      <c r="F9" t="s">
         <v>188</v>
       </c>
-      <c r="G9" s="12" t="s">
+      <c r="G9" t="s">
         <v>189</v>
       </c>
-      <c r="H9" s="23"/>
+      <c r="H9" s="20"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B10" s="22" t="s">
+      <c r="B10" s="19" t="s">
         <v>190</v>
       </c>
-      <c r="C10" s="12" t="s">
+      <c r="C10" t="s">
         <v>191</v>
       </c>
-      <c r="D10" s="12">
+      <c r="D10">
         <v>-3.1680000000000001</v>
       </c>
-      <c r="E10" s="12" t="s">
+      <c r="E10" t="s">
         <v>192</v>
       </c>
-      <c r="F10" s="12" t="s">
+      <c r="F10" t="s">
         <v>193</v>
       </c>
-      <c r="G10" s="12" t="s">
+      <c r="G10" t="s">
         <v>189</v>
       </c>
-      <c r="H10" s="23"/>
+      <c r="H10" s="20"/>
     </row>
     <row r="11" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="40" t="s">
+      <c r="B11" s="23" t="s">
         <v>194</v>
       </c>
-      <c r="C11" s="31" t="s">
+      <c r="C11" s="24" t="s">
         <v>186</v>
       </c>
-      <c r="D11" s="31">
+      <c r="D11" s="24">
         <v>-27933.45</v>
       </c>
-      <c r="E11" s="31" t="s">
+      <c r="E11" s="24" t="s">
         <v>195</v>
       </c>
-      <c r="F11" s="31" t="s">
+      <c r="F11" s="24" t="s">
         <v>188</v>
       </c>
-      <c r="G11" s="31" t="s">
+      <c r="G11" s="24" t="s">
         <v>189</v>
       </c>
-      <c r="H11" s="41"/>
+      <c r="H11" s="26"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B12" s="60" t="s">
+      <c r="B12" s="46" t="s">
         <v>217</v>
       </c>
-      <c r="C12" s="61"/>
-      <c r="D12" s="61"/>
-      <c r="E12" s="61"/>
-      <c r="F12" s="61"/>
-      <c r="G12" s="61"/>
-      <c r="H12" s="62"/>
+      <c r="C12" s="47"/>
+      <c r="D12" s="47"/>
+      <c r="E12" s="47"/>
+      <c r="F12" s="47"/>
+      <c r="G12" s="47"/>
+      <c r="H12" s="48"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B13" s="22" t="s">
+      <c r="B13" s="19" t="s">
         <v>179</v>
       </c>
-      <c r="C13" s="12" t="s">
+      <c r="C13" t="s">
         <v>180</v>
       </c>
-      <c r="D13" s="12" t="s">
+      <c r="D13" t="s">
         <v>27</v>
       </c>
-      <c r="E13" s="12" t="s">
+      <c r="E13" t="s">
         <v>28</v>
       </c>
-      <c r="F13" s="12" t="s">
+      <c r="F13" t="s">
         <v>48</v>
       </c>
-      <c r="G13" s="12" t="s">
+      <c r="G13" t="s">
         <v>181</v>
       </c>
-      <c r="H13" s="23" t="s">
+      <c r="H13" s="20" t="s">
         <v>197</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B14" s="22" t="s">
+      <c r="B14" s="19" t="s">
         <v>196</v>
       </c>
-      <c r="C14" s="12">
+      <c r="C14">
         <v>1</v>
       </c>
-      <c r="D14" s="12">
+      <c r="D14">
         <v>-350734933</v>
       </c>
-      <c r="E14" s="47" t="s">
+      <c r="E14" s="35" t="s">
         <v>198</v>
       </c>
-      <c r="F14" s="12" t="s">
+      <c r="F14" t="s">
         <v>199</v>
       </c>
-      <c r="G14" s="12" t="s">
+      <c r="G14" t="s">
         <v>200</v>
       </c>
-      <c r="H14" s="23">
+      <c r="H14" s="20">
         <v>0.66420000000000001</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B15" s="22" t="s">
+      <c r="B15" s="19" t="s">
         <v>201</v>
       </c>
-      <c r="C15" s="12"/>
-      <c r="D15" s="12">
+      <c r="D15">
         <v>20</v>
       </c>
-      <c r="E15" s="12" t="s">
+      <c r="E15" t="s">
         <v>39</v>
       </c>
-      <c r="F15" s="12"/>
-      <c r="G15" s="12"/>
-      <c r="H15" s="23"/>
+      <c r="H15" s="20"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B16" s="22" t="s">
+      <c r="B16" s="19" t="s">
         <v>202</v>
       </c>
-      <c r="C16" s="12">
+      <c r="C16">
         <v>1</v>
       </c>
-      <c r="D16" s="12">
+      <c r="D16">
         <v>-27412351</v>
       </c>
-      <c r="E16" s="12" t="s">
+      <c r="E16" t="s">
         <v>203</v>
       </c>
-      <c r="F16" s="12" t="s">
+      <c r="F16" t="s">
         <v>188</v>
       </c>
-      <c r="G16" s="12" t="s">
+      <c r="G16" t="s">
         <v>189</v>
       </c>
-      <c r="H16" s="23"/>
+      <c r="H16" s="20"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B17" s="22" t="s">
+      <c r="B17" s="19" t="s">
         <v>204</v>
       </c>
-      <c r="C17" s="12">
+      <c r="C17">
         <v>1</v>
       </c>
-      <c r="D17" s="12">
+      <c r="D17">
         <v>-9636868</v>
       </c>
-      <c r="E17" s="12" t="s">
+      <c r="E17" t="s">
         <v>203</v>
       </c>
-      <c r="F17" s="12" t="s">
+      <c r="F17" t="s">
         <v>188</v>
       </c>
-      <c r="G17" s="12" t="s">
+      <c r="G17" t="s">
         <v>189</v>
       </c>
-      <c r="H17" s="23"/>
+      <c r="H17" s="20"/>
     </row>
     <row r="18" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="48" t="s">
+      <c r="B18" s="36" t="s">
         <v>207</v>
       </c>
-      <c r="C18" s="31" t="s">
+      <c r="C18" s="24" t="s">
         <v>205</v>
       </c>
-      <c r="D18" s="31">
+      <c r="D18" s="24">
         <v>0.13100999999999999</v>
       </c>
-      <c r="E18" s="31" t="s">
+      <c r="E18" s="24" t="s">
         <v>206</v>
       </c>
-      <c r="F18" s="31" t="s">
+      <c r="F18" s="24" t="s">
         <v>193</v>
       </c>
-      <c r="G18" s="31" t="s">
+      <c r="G18" s="24" t="s">
         <v>189</v>
       </c>
-      <c r="H18" s="41"/>
-      <c r="I18" s="49" t="s">
+      <c r="H18" s="26"/>
+      <c r="I18" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A21" s="60" t="s">
+      <c r="A21" s="46" t="s">
         <v>209</v>
       </c>
-      <c r="B21" s="61"/>
-      <c r="C21" s="61"/>
-      <c r="D21" s="62"/>
-      <c r="G21" s="60" t="s">
+      <c r="B21" s="47"/>
+      <c r="C21" s="47"/>
+      <c r="D21" s="48"/>
+      <c r="G21" s="46" t="s">
         <v>214</v>
       </c>
-      <c r="H21" s="62"/>
+      <c r="H21" s="48"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A22" s="22" t="s">
+      <c r="A22" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="B22" s="12" t="s">
+      <c r="B22" t="s">
         <v>210</v>
       </c>
-      <c r="C22" s="12" t="s">
+      <c r="C22" t="s">
         <v>208</v>
       </c>
-      <c r="D22" s="23" t="s">
+      <c r="D22" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="G22" s="22" t="s">
+      <c r="G22" s="19" t="s">
         <v>210</v>
       </c>
-      <c r="H22" s="23" t="s">
+      <c r="H22" s="20" t="s">
         <v>208</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A23" s="22" t="s">
+      <c r="A23" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="B23" s="12" t="s">
+      <c r="B23" t="s">
         <v>174</v>
       </c>
-      <c r="C23" s="12">
+      <c r="C23">
         <v>-1</v>
       </c>
-      <c r="D23" s="23" t="s">
+      <c r="D23" s="20" t="s">
         <v>215</v>
       </c>
-      <c r="G23" s="22" t="s">
+      <c r="G23" s="19" t="s">
         <v>174</v>
       </c>
-      <c r="H23" s="45">
+      <c r="H23" s="33">
         <v>-1</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A24" s="22" t="s">
+      <c r="A24" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="B24" s="12" t="s">
+      <c r="B24" t="s">
         <v>205</v>
       </c>
-      <c r="C24" s="12">
+      <c r="C24">
         <v>25.13</v>
       </c>
-      <c r="D24" s="23" t="s">
+      <c r="D24" s="20" t="s">
         <v>216</v>
       </c>
-      <c r="G24" s="22" t="s">
+      <c r="G24" s="19" t="s">
         <v>211</v>
       </c>
-      <c r="H24" s="45">
+      <c r="H24" s="33">
         <f>(C26/ABS(C$25))*(C$24)</f>
         <v>17.377632075471695</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A25" s="22" t="s">
+      <c r="A25" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="B25" s="12" t="s">
+      <c r="B25" t="s">
         <v>205</v>
       </c>
-      <c r="C25" s="12">
+      <c r="C25">
         <v>-1.06</v>
       </c>
-      <c r="D25" s="23" t="s">
+      <c r="D25" s="20" t="s">
         <v>216</v>
       </c>
-      <c r="G25" s="22" t="s">
+      <c r="G25" s="19" t="s">
         <v>212</v>
       </c>
-      <c r="H25" s="45">
+      <c r="H25" s="33">
         <f>(C27/ABS(C$25))*(C$24)</f>
         <v>21.052301886792449</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="22" t="s">
+      <c r="A26" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="B26" s="12" t="s">
+      <c r="B26" t="s">
         <v>211</v>
       </c>
-      <c r="C26" s="12">
+      <c r="C26">
         <v>0.73299999999999998</v>
       </c>
-      <c r="D26" s="23" t="s">
+      <c r="D26" s="20" t="s">
         <v>216</v>
       </c>
-      <c r="G26" s="40" t="s">
+      <c r="G26" s="23" t="s">
         <v>213</v>
       </c>
-      <c r="H26" s="46">
+      <c r="H26" s="34">
         <f>(C28/ABS(C$25))*(C$24)</f>
         <v>11.664113207547167</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A27" s="22" t="s">
+      <c r="A27" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="B27" s="12" t="s">
+      <c r="B27" t="s">
         <v>212</v>
       </c>
-      <c r="C27" s="12">
+      <c r="C27">
         <v>0.88800000000000001</v>
       </c>
-      <c r="D27" s="23" t="s">
+      <c r="D27" s="20" t="s">
         <v>216</v>
       </c>
     </row>
     <row r="28" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="40" t="s">
+      <c r="A28" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="B28" s="31" t="s">
+      <c r="B28" s="24" t="s">
         <v>213</v>
       </c>
-      <c r="C28" s="31">
+      <c r="C28" s="24">
         <v>0.49199999999999999</v>
       </c>
-      <c r="D28" s="41" t="s">
+      <c r="D28" s="26" t="s">
         <v>216</v>
       </c>
     </row>

</xml_diff>